<commit_message>
Modified test to produce PDF format of W&S BIll.
</commit_message>
<xml_diff>
--- a/tests/modern_wns_bill.xlsx
+++ b/tests/modern_wns_bill.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23980" yWindow="260" windowWidth="24620" windowHeight="22780" tabRatio="752" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="23980" yWindow="240" windowWidth="24620" windowHeight="22780" tabRatio="752" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="9" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3809" uniqueCount="436">
   <si>
     <t>WATCH AND STATION BILL</t>
   </si>
@@ -1509,6 +1509,9 @@
   <si>
     <t>SPECIAL SEA DUTIES</t>
   </si>
+  <si>
+    <t>Damage/Flooding</t>
+  </si>
 </sst>
 </file>
 
@@ -2382,8 +2385,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="291">
+  <cellStyleXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3252,110 +3259,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3402,8 +3305,112 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="291">
+  <cellStyles count="295">
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
@@ -3549,6 +3556,8 @@
     <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
@@ -3694,54 +3703,11 @@
     <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="52">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -4020,6 +3986,51 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
@@ -4102,7 +4113,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17175,34 +17186,34 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1"/>
     <row r="2" spans="2:10" s="10" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B2" s="270" t="s">
+      <c r="B2" s="287" t="s">
         <v>387</v>
       </c>
-      <c r="C2" s="271"/>
+      <c r="C2" s="288"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="274" t="s">
+      <c r="E2" s="291" t="s">
         <v>388</v>
       </c>
-      <c r="F2" s="271"/>
-      <c r="G2" s="275"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="292"/>
       <c r="I2" s="74"/>
       <c r="J2" s="75"/>
     </row>
     <row r="3" spans="2:10" s="10" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="B3" s="272"/>
-      <c r="C3" s="273"/>
+      <c r="B3" s="289"/>
+      <c r="C3" s="290"/>
       <c r="D3" s="13"/>
-      <c r="E3" s="272"/>
-      <c r="F3" s="273"/>
-      <c r="G3" s="276"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="293"/>
       <c r="I3" s="76"/>
       <c r="J3" s="75"/>
     </row>
     <row r="4" spans="2:10" s="17" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B4" s="255" t="s">
+      <c r="B4" s="294" t="s">
         <v>389</v>
       </c>
-      <c r="C4" s="256"/>
+      <c r="C4" s="295"/>
       <c r="D4" s="37"/>
       <c r="E4" s="55"/>
       <c r="F4" s="37"/>
@@ -17211,38 +17222,38 @@
       <c r="J4" s="195"/>
     </row>
     <row r="5" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B5" s="258" t="s">
+      <c r="B5" s="283" t="s">
         <v>390</v>
       </c>
-      <c r="C5" s="259"/>
+      <c r="C5" s="285"/>
       <c r="D5" s="22"/>
-      <c r="E5" s="277" t="s">
+      <c r="E5" s="296" t="s">
         <v>391</v>
       </c>
-      <c r="F5" s="278"/>
-      <c r="G5" s="279"/>
+      <c r="F5" s="297"/>
+      <c r="G5" s="298"/>
       <c r="I5" s="75"/>
       <c r="J5" s="75"/>
     </row>
     <row r="6" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B6" s="260"/>
-      <c r="C6" s="261"/>
+      <c r="B6" s="272"/>
+      <c r="C6" s="271"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="280"/>
-      <c r="F6" s="281"/>
-      <c r="G6" s="282"/>
+      <c r="E6" s="299"/>
+      <c r="F6" s="300"/>
+      <c r="G6" s="301"/>
       <c r="I6" s="77"/>
-      <c r="J6" s="257"/>
+      <c r="J6" s="302"/>
     </row>
     <row r="7" spans="2:10" ht="15.5" customHeight="1" thickBot="1">
-      <c r="B7" s="260"/>
-      <c r="C7" s="261"/>
+      <c r="B7" s="272"/>
+      <c r="C7" s="271"/>
       <c r="D7" s="26"/>
-      <c r="E7" s="280"/>
-      <c r="F7" s="281"/>
-      <c r="G7" s="282"/>
+      <c r="E7" s="299"/>
+      <c r="F7" s="300"/>
+      <c r="G7" s="301"/>
       <c r="I7" s="75"/>
-      <c r="J7" s="257"/>
+      <c r="J7" s="302"/>
     </row>
     <row r="8" spans="2:10" ht="15.5" customHeight="1">
       <c r="B8" s="48" t="s">
@@ -17250,47 +17261,47 @@
       </c>
       <c r="C8" s="50"/>
       <c r="D8" s="26"/>
-      <c r="E8" s="258" t="s">
+      <c r="E8" s="283" t="s">
         <v>393</v>
       </c>
-      <c r="F8" s="283"/>
-      <c r="G8" s="259"/>
+      <c r="F8" s="284"/>
+      <c r="G8" s="285"/>
       <c r="I8" s="75"/>
-      <c r="J8" s="257"/>
+      <c r="J8" s="302"/>
     </row>
     <row r="9" spans="2:10" ht="15.5" customHeight="1" thickBot="1">
       <c r="B9" s="52"/>
       <c r="C9" s="54"/>
       <c r="D9" s="26"/>
-      <c r="E9" s="267"/>
-      <c r="F9" s="268"/>
-      <c r="G9" s="269"/>
+      <c r="E9" s="275"/>
+      <c r="F9" s="276"/>
+      <c r="G9" s="277"/>
       <c r="I9" s="75"/>
-      <c r="J9" s="257"/>
+      <c r="J9" s="302"/>
     </row>
     <row r="10" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="281" t="s">
         <v>394</v>
       </c>
-      <c r="C10" s="265"/>
+      <c r="C10" s="282"/>
       <c r="D10" s="26"/>
-      <c r="E10" s="258" t="s">
+      <c r="E10" s="283" t="s">
         <v>395</v>
       </c>
-      <c r="F10" s="283"/>
-      <c r="G10" s="259"/>
+      <c r="F10" s="284"/>
+      <c r="G10" s="285"/>
       <c r="I10" s="75"/>
       <c r="J10" s="75"/>
     </row>
     <row r="11" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B11" s="262" t="s">
+      <c r="B11" s="273" t="s">
         <v>396</v>
       </c>
-      <c r="C11" s="263"/>
+      <c r="C11" s="274"/>
       <c r="D11" s="26"/>
-      <c r="E11" s="260"/>
-      <c r="F11" s="266"/>
-      <c r="G11" s="261"/>
+      <c r="E11" s="272"/>
+      <c r="F11" s="270"/>
+      <c r="G11" s="271"/>
       <c r="I11" s="75"/>
       <c r="J11" s="195"/>
     </row>
@@ -17298,130 +17309,130 @@
       <c r="B12" s="47"/>
       <c r="C12" s="4"/>
       <c r="D12" s="26"/>
-      <c r="E12" s="260"/>
-      <c r="F12" s="266"/>
-      <c r="G12" s="261"/>
+      <c r="E12" s="272"/>
+      <c r="F12" s="270"/>
+      <c r="G12" s="271"/>
       <c r="I12" s="77"/>
       <c r="J12" s="75"/>
     </row>
     <row r="13" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B13" s="262" t="s">
+      <c r="B13" s="273" t="s">
         <v>397</v>
       </c>
-      <c r="C13" s="263"/>
+      <c r="C13" s="274"/>
       <c r="D13" s="26"/>
-      <c r="E13" s="258" t="s">
+      <c r="E13" s="283" t="s">
         <v>398</v>
       </c>
-      <c r="F13" s="283"/>
-      <c r="G13" s="259"/>
+      <c r="F13" s="284"/>
+      <c r="G13" s="285"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="2:10" ht="15.5" customHeight="1">
       <c r="B14" s="47"/>
       <c r="D14" s="26"/>
-      <c r="E14" s="260"/>
-      <c r="F14" s="284"/>
-      <c r="G14" s="261"/>
+      <c r="E14" s="272"/>
+      <c r="F14" s="286"/>
+      <c r="G14" s="271"/>
     </row>
     <row r="15" spans="2:10" ht="15.5" customHeight="1">
-      <c r="B15" s="262" t="s">
+      <c r="B15" s="273" t="s">
         <v>399</v>
       </c>
-      <c r="C15" s="263"/>
+      <c r="C15" s="274"/>
       <c r="D15" s="26"/>
-      <c r="E15" s="260"/>
-      <c r="F15" s="284"/>
-      <c r="G15" s="261"/>
+      <c r="E15" s="272"/>
+      <c r="F15" s="286"/>
+      <c r="G15" s="271"/>
     </row>
     <row r="16" spans="2:10" ht="15.5" customHeight="1">
       <c r="B16" s="12"/>
       <c r="C16" s="51"/>
       <c r="D16" s="26"/>
-      <c r="E16" s="285" t="s">
+      <c r="E16" s="269" t="s">
         <v>400</v>
       </c>
-      <c r="F16" s="266"/>
-      <c r="G16" s="261"/>
+      <c r="F16" s="270"/>
+      <c r="G16" s="271"/>
     </row>
     <row r="17" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B17" s="262" t="s">
+      <c r="B17" s="273" t="s">
         <v>401</v>
       </c>
-      <c r="C17" s="263"/>
+      <c r="C17" s="274"/>
       <c r="D17" s="26"/>
-      <c r="E17" s="260"/>
-      <c r="F17" s="266"/>
-      <c r="G17" s="261"/>
+      <c r="E17" s="272"/>
+      <c r="F17" s="270"/>
+      <c r="G17" s="271"/>
     </row>
     <row r="18" spans="1:8" ht="15.5" customHeight="1">
       <c r="B18" s="12"/>
       <c r="C18" s="51"/>
       <c r="D18" s="26"/>
-      <c r="E18" s="260"/>
-      <c r="F18" s="266"/>
-      <c r="G18" s="261"/>
+      <c r="E18" s="272"/>
+      <c r="F18" s="270"/>
+      <c r="G18" s="271"/>
     </row>
     <row r="19" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B19" s="262" t="s">
+      <c r="B19" s="273" t="s">
         <v>402</v>
       </c>
-      <c r="C19" s="263"/>
+      <c r="C19" s="274"/>
       <c r="D19" s="26"/>
-      <c r="E19" s="260" t="s">
+      <c r="E19" s="272" t="s">
         <v>403</v>
       </c>
-      <c r="F19" s="266"/>
-      <c r="G19" s="261"/>
+      <c r="F19" s="270"/>
+      <c r="G19" s="271"/>
     </row>
     <row r="20" spans="1:8" ht="15.5" customHeight="1">
       <c r="B20" s="12"/>
       <c r="C20" s="51"/>
       <c r="D20" s="26"/>
-      <c r="E20" s="260"/>
-      <c r="F20" s="266"/>
-      <c r="G20" s="261"/>
+      <c r="E20" s="272"/>
+      <c r="F20" s="270"/>
+      <c r="G20" s="271"/>
     </row>
     <row r="21" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="B21" s="52"/>
       <c r="C21" s="54"/>
       <c r="D21" s="32"/>
-      <c r="E21" s="267"/>
-      <c r="F21" s="268"/>
-      <c r="G21" s="269"/>
+      <c r="E21" s="275"/>
+      <c r="F21" s="276"/>
+      <c r="G21" s="277"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1"/>
     <row r="25" spans="1:8">
       <c r="A25" s="10"/>
-      <c r="B25" s="270" t="s">
+      <c r="B25" s="287" t="s">
         <v>404</v>
       </c>
-      <c r="C25" s="271"/>
+      <c r="C25" s="288"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="274" t="s">
+      <c r="E25" s="291" t="s">
         <v>405</v>
       </c>
-      <c r="F25" s="271"/>
-      <c r="G25" s="275"/>
+      <c r="F25" s="288"/>
+      <c r="G25" s="292"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" ht="25.5" customHeight="1" thickBot="1">
       <c r="A26" s="10"/>
-      <c r="B26" s="272"/>
-      <c r="C26" s="273"/>
+      <c r="B26" s="289"/>
+      <c r="C26" s="290"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="272"/>
-      <c r="F26" s="273"/>
-      <c r="G26" s="276"/>
+      <c r="E26" s="289"/>
+      <c r="F26" s="290"/>
+      <c r="G26" s="293"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="A27" s="17"/>
-      <c r="B27" s="255" t="s">
+      <c r="B27" s="294" t="s">
         <v>406</v>
       </c>
-      <c r="C27" s="256"/>
+      <c r="C27" s="295"/>
       <c r="D27" s="37"/>
       <c r="E27" s="55"/>
       <c r="F27" s="37"/>
@@ -17429,32 +17440,32 @@
       <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B28" s="258" t="s">
+      <c r="B28" s="283" t="s">
         <v>390</v>
       </c>
-      <c r="C28" s="259"/>
+      <c r="C28" s="285"/>
       <c r="D28" s="22"/>
-      <c r="E28" s="277" t="s">
+      <c r="E28" s="296" t="s">
         <v>391</v>
       </c>
-      <c r="F28" s="278"/>
-      <c r="G28" s="279"/>
+      <c r="F28" s="297"/>
+      <c r="G28" s="298"/>
     </row>
     <row r="29" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B29" s="260"/>
-      <c r="C29" s="261"/>
+      <c r="B29" s="272"/>
+      <c r="C29" s="271"/>
       <c r="D29" s="26"/>
-      <c r="E29" s="280"/>
-      <c r="F29" s="281"/>
-      <c r="G29" s="282"/>
+      <c r="E29" s="299"/>
+      <c r="F29" s="300"/>
+      <c r="G29" s="301"/>
     </row>
     <row r="30" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
-      <c r="B30" s="260"/>
-      <c r="C30" s="261"/>
+      <c r="B30" s="272"/>
+      <c r="C30" s="271"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="280"/>
-      <c r="F30" s="281"/>
-      <c r="G30" s="282"/>
+      <c r="E30" s="299"/>
+      <c r="F30" s="300"/>
+      <c r="G30" s="301"/>
     </row>
     <row r="31" spans="1:8" ht="15.5" customHeight="1">
       <c r="B31" s="48" t="s">
@@ -17462,201 +17473,201 @@
       </c>
       <c r="C31" s="50"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="258" t="s">
+      <c r="E31" s="283" t="s">
         <v>393</v>
       </c>
-      <c r="F31" s="283"/>
-      <c r="G31" s="259"/>
+      <c r="F31" s="284"/>
+      <c r="G31" s="285"/>
     </row>
     <row r="32" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="B32" s="52"/>
       <c r="C32" s="54"/>
       <c r="D32" s="26"/>
-      <c r="E32" s="267"/>
-      <c r="F32" s="268"/>
-      <c r="G32" s="269"/>
+      <c r="E32" s="275"/>
+      <c r="F32" s="276"/>
+      <c r="G32" s="277"/>
     </row>
     <row r="33" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B33" s="264" t="s">
+      <c r="B33" s="281" t="s">
         <v>394</v>
       </c>
-      <c r="C33" s="265"/>
+      <c r="C33" s="282"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="258" t="s">
+      <c r="E33" s="283" t="s">
         <v>395</v>
       </c>
-      <c r="F33" s="283"/>
-      <c r="G33" s="259"/>
+      <c r="F33" s="284"/>
+      <c r="G33" s="285"/>
     </row>
     <row r="34" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B34" s="262" t="s">
+      <c r="B34" s="273" t="s">
         <v>396</v>
       </c>
-      <c r="C34" s="263"/>
+      <c r="C34" s="274"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="260"/>
-      <c r="F34" s="266"/>
-      <c r="G34" s="261"/>
+      <c r="E34" s="272"/>
+      <c r="F34" s="270"/>
+      <c r="G34" s="271"/>
     </row>
     <row r="35" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="B35" s="47"/>
       <c r="C35" s="4"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="260"/>
-      <c r="F35" s="266"/>
-      <c r="G35" s="261"/>
+      <c r="E35" s="272"/>
+      <c r="F35" s="270"/>
+      <c r="G35" s="271"/>
     </row>
     <row r="36" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B36" s="262" t="s">
+      <c r="B36" s="273" t="s">
         <v>397</v>
       </c>
-      <c r="C36" s="263"/>
+      <c r="C36" s="274"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="258" t="s">
+      <c r="E36" s="283" t="s">
         <v>398</v>
       </c>
-      <c r="F36" s="283"/>
-      <c r="G36" s="259"/>
+      <c r="F36" s="284"/>
+      <c r="G36" s="285"/>
     </row>
     <row r="37" spans="1:8" ht="15.5" customHeight="1">
       <c r="B37" s="47"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="260"/>
-      <c r="F37" s="284"/>
-      <c r="G37" s="261"/>
+      <c r="E37" s="272"/>
+      <c r="F37" s="286"/>
+      <c r="G37" s="271"/>
     </row>
     <row r="38" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B38" s="262" t="s">
+      <c r="B38" s="273" t="s">
         <v>399</v>
       </c>
-      <c r="C38" s="263"/>
+      <c r="C38" s="274"/>
       <c r="D38" s="26"/>
-      <c r="E38" s="260"/>
-      <c r="F38" s="284"/>
-      <c r="G38" s="261"/>
+      <c r="E38" s="272"/>
+      <c r="F38" s="286"/>
+      <c r="G38" s="271"/>
     </row>
     <row r="39" spans="1:8" ht="15.5" customHeight="1">
       <c r="B39" s="12"/>
       <c r="C39" s="51"/>
       <c r="D39" s="26"/>
-      <c r="E39" s="285" t="s">
+      <c r="E39" s="269" t="s">
         <v>400</v>
       </c>
-      <c r="F39" s="266"/>
-      <c r="G39" s="261"/>
+      <c r="F39" s="270"/>
+      <c r="G39" s="271"/>
     </row>
     <row r="40" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B40" s="262" t="s">
+      <c r="B40" s="273" t="s">
         <v>401</v>
       </c>
-      <c r="C40" s="263"/>
+      <c r="C40" s="274"/>
       <c r="D40" s="26"/>
-      <c r="E40" s="260"/>
-      <c r="F40" s="266"/>
-      <c r="G40" s="261"/>
+      <c r="E40" s="272"/>
+      <c r="F40" s="270"/>
+      <c r="G40" s="271"/>
     </row>
     <row r="41" spans="1:8" ht="15.5" customHeight="1">
       <c r="B41" s="12"/>
       <c r="C41" s="51"/>
       <c r="D41" s="26"/>
-      <c r="E41" s="260"/>
-      <c r="F41" s="266"/>
-      <c r="G41" s="261"/>
+      <c r="E41" s="272"/>
+      <c r="F41" s="270"/>
+      <c r="G41" s="271"/>
     </row>
     <row r="42" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B42" s="262" t="s">
+      <c r="B42" s="273" t="s">
         <v>402</v>
       </c>
-      <c r="C42" s="263"/>
+      <c r="C42" s="274"/>
       <c r="D42" s="26"/>
-      <c r="E42" s="260" t="s">
+      <c r="E42" s="272" t="s">
         <v>403</v>
       </c>
-      <c r="F42" s="266"/>
-      <c r="G42" s="261"/>
+      <c r="F42" s="270"/>
+      <c r="G42" s="271"/>
     </row>
     <row r="43" spans="1:8" ht="15.5" customHeight="1">
       <c r="B43" s="12"/>
       <c r="C43" s="51"/>
       <c r="D43" s="26"/>
-      <c r="E43" s="260"/>
-      <c r="F43" s="266"/>
-      <c r="G43" s="261"/>
+      <c r="E43" s="272"/>
+      <c r="F43" s="270"/>
+      <c r="G43" s="271"/>
     </row>
     <row r="44" spans="1:8" ht="15" thickBot="1">
       <c r="B44" s="52"/>
       <c r="C44" s="54"/>
       <c r="D44" s="32"/>
-      <c r="E44" s="267"/>
-      <c r="F44" s="268"/>
-      <c r="G44" s="269"/>
+      <c r="E44" s="275"/>
+      <c r="F44" s="276"/>
+      <c r="G44" s="277"/>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1"/>
     <row r="47" spans="1:8">
       <c r="A47" s="10"/>
-      <c r="B47" s="270" t="s">
+      <c r="B47" s="287" t="s">
         <v>407</v>
       </c>
-      <c r="C47" s="271"/>
+      <c r="C47" s="288"/>
       <c r="D47" s="7"/>
-      <c r="E47" s="274" t="s">
+      <c r="E47" s="291" t="s">
         <v>408</v>
       </c>
-      <c r="F47" s="271"/>
-      <c r="G47" s="275"/>
+      <c r="F47" s="288"/>
+      <c r="G47" s="292"/>
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8" ht="15" thickBot="1">
       <c r="A48" s="10"/>
-      <c r="B48" s="272"/>
-      <c r="C48" s="273"/>
+      <c r="B48" s="289"/>
+      <c r="C48" s="290"/>
       <c r="D48" s="13"/>
-      <c r="E48" s="272"/>
-      <c r="F48" s="273"/>
-      <c r="G48" s="276"/>
+      <c r="E48" s="289"/>
+      <c r="F48" s="290"/>
+      <c r="G48" s="293"/>
       <c r="H48" s="10"/>
     </row>
     <row r="49" spans="1:8" ht="30.75" customHeight="1" thickBot="1">
       <c r="A49" s="17"/>
-      <c r="B49" s="255" t="s">
+      <c r="B49" s="294" t="s">
         <v>409</v>
       </c>
-      <c r="C49" s="256"/>
+      <c r="C49" s="295"/>
       <c r="D49" s="37"/>
-      <c r="E49" s="286" t="s">
+      <c r="E49" s="278" t="s">
         <v>410</v>
       </c>
-      <c r="F49" s="287"/>
-      <c r="G49" s="288"/>
+      <c r="F49" s="279"/>
+      <c r="G49" s="280"/>
       <c r="H49" s="17"/>
     </row>
     <row r="50" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B50" s="258" t="s">
+      <c r="B50" s="283" t="s">
         <v>390</v>
       </c>
-      <c r="C50" s="259"/>
+      <c r="C50" s="285"/>
       <c r="D50" s="22"/>
-      <c r="E50" s="277" t="s">
+      <c r="E50" s="296" t="s">
         <v>411</v>
       </c>
-      <c r="F50" s="278"/>
-      <c r="G50" s="279"/>
+      <c r="F50" s="297"/>
+      <c r="G50" s="298"/>
     </row>
     <row r="51" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B51" s="260"/>
-      <c r="C51" s="261"/>
+      <c r="B51" s="272"/>
+      <c r="C51" s="271"/>
       <c r="D51" s="26"/>
-      <c r="E51" s="280"/>
-      <c r="F51" s="281"/>
-      <c r="G51" s="282"/>
+      <c r="E51" s="299"/>
+      <c r="F51" s="300"/>
+      <c r="G51" s="301"/>
     </row>
     <row r="52" spans="1:8" ht="8.25" customHeight="1" thickBot="1">
-      <c r="B52" s="260"/>
-      <c r="C52" s="261"/>
+      <c r="B52" s="272"/>
+      <c r="C52" s="271"/>
       <c r="D52" s="26"/>
-      <c r="E52" s="280"/>
-      <c r="F52" s="281"/>
-      <c r="G52" s="282"/>
+      <c r="E52" s="299"/>
+      <c r="F52" s="300"/>
+      <c r="G52" s="301"/>
     </row>
     <row r="53" spans="1:8" ht="15.5" customHeight="1">
       <c r="B53" s="48" t="s">
@@ -17664,130 +17675,130 @@
       </c>
       <c r="C53" s="50"/>
       <c r="D53" s="26"/>
-      <c r="E53" s="258" t="s">
+      <c r="E53" s="283" t="s">
         <v>412</v>
       </c>
-      <c r="F53" s="283"/>
-      <c r="G53" s="259"/>
+      <c r="F53" s="284"/>
+      <c r="G53" s="285"/>
     </row>
     <row r="54" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="B54" s="52"/>
       <c r="C54" s="54"/>
       <c r="D54" s="26"/>
-      <c r="E54" s="267"/>
-      <c r="F54" s="268"/>
-      <c r="G54" s="269"/>
+      <c r="E54" s="275"/>
+      <c r="F54" s="276"/>
+      <c r="G54" s="277"/>
     </row>
     <row r="55" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B55" s="264" t="s">
+      <c r="B55" s="281" t="s">
         <v>413</v>
       </c>
-      <c r="C55" s="265"/>
+      <c r="C55" s="282"/>
       <c r="D55" s="26"/>
-      <c r="E55" s="258" t="s">
+      <c r="E55" s="283" t="s">
         <v>414</v>
       </c>
-      <c r="F55" s="283"/>
-      <c r="G55" s="259"/>
+      <c r="F55" s="284"/>
+      <c r="G55" s="285"/>
     </row>
     <row r="56" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B56" s="262" t="s">
+      <c r="B56" s="273" t="s">
         <v>396</v>
       </c>
-      <c r="C56" s="263"/>
+      <c r="C56" s="274"/>
       <c r="D56" s="26"/>
-      <c r="E56" s="260"/>
-      <c r="F56" s="266"/>
-      <c r="G56" s="261"/>
+      <c r="E56" s="272"/>
+      <c r="F56" s="270"/>
+      <c r="G56" s="271"/>
     </row>
     <row r="57" spans="1:8" ht="15.5" customHeight="1" thickBot="1">
       <c r="B57" s="47"/>
       <c r="C57" s="4"/>
       <c r="D57" s="26"/>
-      <c r="E57" s="260"/>
-      <c r="F57" s="266"/>
-      <c r="G57" s="261"/>
+      <c r="E57" s="272"/>
+      <c r="F57" s="270"/>
+      <c r="G57" s="271"/>
     </row>
     <row r="58" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B58" s="262" t="s">
+      <c r="B58" s="273" t="s">
         <v>397</v>
       </c>
-      <c r="C58" s="263"/>
+      <c r="C58" s="274"/>
       <c r="D58" s="26"/>
-      <c r="E58" s="258" t="s">
+      <c r="E58" s="283" t="s">
         <v>415</v>
       </c>
-      <c r="F58" s="283"/>
-      <c r="G58" s="259"/>
+      <c r="F58" s="284"/>
+      <c r="G58" s="285"/>
     </row>
     <row r="59" spans="1:8" ht="15.5" customHeight="1">
       <c r="B59" s="47"/>
       <c r="D59" s="26"/>
-      <c r="E59" s="260"/>
-      <c r="F59" s="284"/>
-      <c r="G59" s="261"/>
+      <c r="E59" s="272"/>
+      <c r="F59" s="286"/>
+      <c r="G59" s="271"/>
     </row>
     <row r="60" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B60" s="262" t="s">
+      <c r="B60" s="273" t="s">
         <v>399</v>
       </c>
-      <c r="C60" s="263"/>
+      <c r="C60" s="274"/>
       <c r="D60" s="26"/>
-      <c r="E60" s="260"/>
-      <c r="F60" s="284"/>
-      <c r="G60" s="261"/>
+      <c r="E60" s="272"/>
+      <c r="F60" s="286"/>
+      <c r="G60" s="271"/>
     </row>
     <row r="61" spans="1:8" ht="15.5" customHeight="1">
       <c r="B61" s="12"/>
       <c r="C61" s="51"/>
       <c r="D61" s="26"/>
-      <c r="E61" s="285"/>
-      <c r="F61" s="266"/>
-      <c r="G61" s="261"/>
+      <c r="E61" s="269"/>
+      <c r="F61" s="270"/>
+      <c r="G61" s="271"/>
     </row>
     <row r="62" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B62" s="262" t="s">
+      <c r="B62" s="273" t="s">
         <v>401</v>
       </c>
-      <c r="C62" s="263"/>
+      <c r="C62" s="274"/>
       <c r="D62" s="26"/>
-      <c r="E62" s="260"/>
-      <c r="F62" s="266"/>
-      <c r="G62" s="261"/>
+      <c r="E62" s="272"/>
+      <c r="F62" s="270"/>
+      <c r="G62" s="271"/>
     </row>
     <row r="63" spans="1:8" ht="15.5" customHeight="1">
       <c r="B63" s="12"/>
       <c r="C63" s="51"/>
       <c r="D63" s="26"/>
-      <c r="E63" s="260"/>
-      <c r="F63" s="266"/>
-      <c r="G63" s="261"/>
+      <c r="E63" s="272"/>
+      <c r="F63" s="270"/>
+      <c r="G63" s="271"/>
     </row>
     <row r="64" spans="1:8" ht="15.5" customHeight="1">
-      <c r="B64" s="262" t="s">
+      <c r="B64" s="273" t="s">
         <v>402</v>
       </c>
-      <c r="C64" s="263"/>
+      <c r="C64" s="274"/>
       <c r="D64" s="26"/>
-      <c r="E64" s="260"/>
-      <c r="F64" s="266"/>
-      <c r="G64" s="261"/>
+      <c r="E64" s="272"/>
+      <c r="F64" s="270"/>
+      <c r="G64" s="271"/>
     </row>
     <row r="65" spans="2:7" ht="15.5" customHeight="1">
       <c r="B65" s="12"/>
       <c r="C65" s="51"/>
       <c r="D65" s="26"/>
-      <c r="E65" s="260"/>
-      <c r="F65" s="266"/>
-      <c r="G65" s="261"/>
+      <c r="E65" s="272"/>
+      <c r="F65" s="270"/>
+      <c r="G65" s="271"/>
     </row>
     <row r="66" spans="2:7" ht="15.5" customHeight="1" thickBot="1">
       <c r="B66" s="52"/>
       <c r="C66" s="54"/>
       <c r="D66" s="32"/>
-      <c r="E66" s="267"/>
-      <c r="F66" s="268"/>
-      <c r="G66" s="269"/>
+      <c r="E66" s="275"/>
+      <c r="F66" s="276"/>
+      <c r="G66" s="277"/>
     </row>
     <row r="67" spans="2:7" ht="15.5" customHeight="1"/>
     <row r="68" spans="2:7" ht="15" thickBot="1"/>
@@ -19897,23 +19908,26 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="E61:G63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="E64:G66"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="E55:G57"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="E58:G60"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="E53:G54"/>
-    <mergeCell ref="B47:C48"/>
-    <mergeCell ref="E47:G48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C52"/>
-    <mergeCell ref="E50:G52"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="B5:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E19:G21"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E2:G3"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="E25:G26"/>
+    <mergeCell ref="E5:G7"/>
+    <mergeCell ref="E8:G9"/>
+    <mergeCell ref="E10:G12"/>
+    <mergeCell ref="E13:G15"/>
+    <mergeCell ref="E16:G18"/>
     <mergeCell ref="B42:C42"/>
     <mergeCell ref="E42:G44"/>
     <mergeCell ref="B28:C30"/>
@@ -19927,26 +19941,23 @@
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="E39:G41"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E2:G3"/>
-    <mergeCell ref="B25:C26"/>
-    <mergeCell ref="E25:G26"/>
-    <mergeCell ref="E5:G7"/>
-    <mergeCell ref="E8:G9"/>
-    <mergeCell ref="E10:G12"/>
-    <mergeCell ref="E13:G15"/>
-    <mergeCell ref="E16:G18"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="B5:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E19:G21"/>
+    <mergeCell ref="B47:C48"/>
+    <mergeCell ref="E47:G48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C52"/>
+    <mergeCell ref="E50:G52"/>
+    <mergeCell ref="E61:G63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="E64:G66"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="E55:G57"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="E58:G60"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="E53:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -19965,9 +19976,9 @@
   </sheetPr>
   <dimension ref="A1:BB178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:BA3"/>
+      <selection pane="bottomLeft" activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -20017,11 +20028,11 @@
       <c r="S1" s="143"/>
       <c r="T1" s="143"/>
       <c r="U1" s="143"/>
-      <c r="V1" s="253" t="s">
+      <c r="V1" s="267" t="s">
         <v>87</v>
       </c>
-      <c r="W1" s="254"/>
-      <c r="X1" s="254"/>
+      <c r="W1" s="268"/>
+      <c r="X1" s="268"/>
       <c r="Y1" s="96"/>
       <c r="Z1" s="96"/>
       <c r="AA1" s="96"/>
@@ -20133,16 +20144,16 @@
       <c r="H3" s="166" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="289" t="s">
+      <c r="I3" s="253" t="s">
         <v>212</v>
       </c>
-      <c r="J3" s="289" t="s">
+      <c r="J3" s="253" t="s">
         <v>317</v>
       </c>
-      <c r="K3" s="289" t="s">
+      <c r="K3" s="253" t="s">
         <v>418</v>
       </c>
-      <c r="L3" s="289" t="s">
+      <c r="L3" s="253" t="s">
         <v>419</v>
       </c>
       <c r="M3" s="167" t="s">
@@ -20170,7 +20181,7 @@
         <v>105</v>
       </c>
       <c r="U3" s="168" t="s">
-        <v>106</v>
+        <v>435</v>
       </c>
       <c r="V3" s="168" t="s">
         <v>107</v>
@@ -20271,9 +20282,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-      <c r="U4" s="148" t="b">
+      <c r="U4" s="148" t="e">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>#N/A</v>
       </c>
       <c r="V4" s="148" t="b">
         <f t="shared" ca="1" si="1"/>
@@ -20327,10 +20338,10 @@
       <c r="F5" s="125"/>
       <c r="G5" s="117"/>
       <c r="H5" s="135"/>
-      <c r="I5" s="290"/>
-      <c r="J5" s="290"/>
-      <c r="K5" s="290"/>
-      <c r="L5" s="290"/>
+      <c r="I5" s="254"/>
+      <c r="J5" s="254"/>
+      <c r="K5" s="254"/>
+      <c r="L5" s="254"/>
       <c r="M5" s="150"/>
       <c r="N5" s="127"/>
       <c r="O5" s="127"/>
@@ -20385,10 +20396,10 @@
       <c r="F6" s="125"/>
       <c r="G6" s="117"/>
       <c r="H6" s="135"/>
-      <c r="I6" s="290"/>
-      <c r="J6" s="290"/>
-      <c r="K6" s="290"/>
-      <c r="L6" s="290"/>
+      <c r="I6" s="254"/>
+      <c r="J6" s="254"/>
+      <c r="K6" s="254"/>
+      <c r="L6" s="254"/>
       <c r="M6" s="152"/>
       <c r="N6" s="153"/>
       <c r="O6" s="153"/>
@@ -20619,10 +20630,10 @@
       <c r="F9" s="111"/>
       <c r="G9" s="111"/>
       <c r="H9" s="139"/>
-      <c r="I9" s="291"/>
-      <c r="J9" s="291"/>
-      <c r="K9" s="291"/>
-      <c r="L9" s="291"/>
+      <c r="I9" s="255"/>
+      <c r="J9" s="255"/>
+      <c r="K9" s="255"/>
+      <c r="L9" s="255"/>
       <c r="M9" s="130"/>
       <c r="N9" s="111"/>
       <c r="O9" s="111"/>
@@ -20681,10 +20692,10 @@
       <c r="F10" s="155"/>
       <c r="G10" s="122"/>
       <c r="H10" s="174"/>
-      <c r="I10" s="292"/>
-      <c r="J10" s="292"/>
-      <c r="K10" s="292"/>
-      <c r="L10" s="292"/>
+      <c r="I10" s="256"/>
+      <c r="J10" s="256"/>
+      <c r="K10" s="256"/>
+      <c r="L10" s="256"/>
       <c r="M10" s="175"/>
       <c r="N10" s="155"/>
       <c r="O10" s="155"/>
@@ -20720,10 +20731,10 @@
       <c r="H11" s="213">
         <v>1</v>
       </c>
-      <c r="I11" s="293"/>
-      <c r="J11" s="293"/>
-      <c r="K11" s="293"/>
-      <c r="L11" s="293"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
+      <c r="L11" s="257"/>
       <c r="M11" s="214" t="s">
         <v>115</v>
       </c>
@@ -20777,10 +20788,10 @@
       <c r="H12" s="213">
         <v>1</v>
       </c>
-      <c r="I12" s="293"/>
-      <c r="J12" s="293"/>
-      <c r="K12" s="293"/>
-      <c r="L12" s="293"/>
+      <c r="I12" s="257"/>
+      <c r="J12" s="257"/>
+      <c r="K12" s="257"/>
+      <c r="L12" s="257"/>
       <c r="M12" s="214" t="s">
         <v>117</v>
       </c>
@@ -20822,10 +20833,10 @@
       <c r="H13" s="213">
         <v>1</v>
       </c>
-      <c r="I13" s="293"/>
-      <c r="J13" s="293"/>
-      <c r="K13" s="293"/>
-      <c r="L13" s="293"/>
+      <c r="I13" s="257"/>
+      <c r="J13" s="257"/>
+      <c r="K13" s="257"/>
+      <c r="L13" s="257"/>
       <c r="M13" s="214" t="s">
         <v>130</v>
       </c>
@@ -20867,10 +20878,10 @@
       <c r="H14" s="213">
         <v>1</v>
       </c>
-      <c r="I14" s="293"/>
-      <c r="J14" s="293"/>
-      <c r="K14" s="293"/>
-      <c r="L14" s="293"/>
+      <c r="I14" s="257"/>
+      <c r="J14" s="257"/>
+      <c r="K14" s="257"/>
+      <c r="L14" s="257"/>
       <c r="M14" s="214" t="s">
         <v>130</v>
       </c>
@@ -20916,10 +20927,10 @@
       <c r="H15" s="213">
         <v>1</v>
       </c>
-      <c r="I15" s="293"/>
-      <c r="J15" s="293"/>
-      <c r="K15" s="293"/>
-      <c r="L15" s="293"/>
+      <c r="I15" s="257"/>
+      <c r="J15" s="257"/>
+      <c r="K15" s="257"/>
+      <c r="L15" s="257"/>
       <c r="M15" s="214" t="s">
         <v>137</v>
       </c>
@@ -20967,10 +20978,10 @@
       <c r="H16" s="213">
         <v>1</v>
       </c>
-      <c r="I16" s="293"/>
-      <c r="J16" s="293"/>
-      <c r="K16" s="293"/>
-      <c r="L16" s="293"/>
+      <c r="I16" s="257"/>
+      <c r="J16" s="257"/>
+      <c r="K16" s="257"/>
+      <c r="L16" s="257"/>
       <c r="M16" s="214" t="s">
         <v>140</v>
       </c>
@@ -21008,10 +21019,10 @@
       <c r="H17" s="213">
         <v>1</v>
       </c>
-      <c r="I17" s="293"/>
-      <c r="J17" s="293"/>
-      <c r="K17" s="293"/>
-      <c r="L17" s="293"/>
+      <c r="I17" s="257"/>
+      <c r="J17" s="257"/>
+      <c r="K17" s="257"/>
+      <c r="L17" s="257"/>
       <c r="M17" s="214" t="s">
         <v>117</v>
       </c>
@@ -21067,10 +21078,10 @@
       <c r="H18" s="220">
         <v>1</v>
       </c>
-      <c r="I18" s="294"/>
-      <c r="J18" s="294"/>
-      <c r="K18" s="294"/>
-      <c r="L18" s="294"/>
+      <c r="I18" s="258"/>
+      <c r="J18" s="258"/>
+      <c r="K18" s="258"/>
+      <c r="L18" s="258"/>
       <c r="M18" s="221" t="s">
         <v>146</v>
       </c>
@@ -21156,10 +21167,10 @@
       <c r="H19" s="213">
         <v>1</v>
       </c>
-      <c r="I19" s="293"/>
-      <c r="J19" s="293"/>
-      <c r="K19" s="293"/>
-      <c r="L19" s="293"/>
+      <c r="I19" s="257"/>
+      <c r="J19" s="257"/>
+      <c r="K19" s="257"/>
+      <c r="L19" s="257"/>
       <c r="M19" s="214" t="s">
         <v>146</v>
       </c>
@@ -21205,14 +21216,14 @@
       <c r="H20" s="213">
         <v>1</v>
       </c>
-      <c r="I20" s="293">
+      <c r="I20" s="257">
         <v>2</v>
       </c>
-      <c r="J20" s="293"/>
-      <c r="K20" s="293">
+      <c r="J20" s="257"/>
+      <c r="K20" s="257">
         <v>5</v>
       </c>
-      <c r="L20" s="293">
+      <c r="L20" s="257">
         <v>1</v>
       </c>
       <c r="M20" s="214" t="s">
@@ -21262,12 +21273,12 @@
       <c r="H21" s="213">
         <v>1</v>
       </c>
-      <c r="I21" s="293">
+      <c r="I21" s="257">
         <v>5</v>
       </c>
-      <c r="J21" s="293"/>
-      <c r="K21" s="293"/>
-      <c r="L21" s="293">
+      <c r="J21" s="257"/>
+      <c r="K21" s="257"/>
+      <c r="L21" s="257">
         <v>2</v>
       </c>
       <c r="M21" s="214" t="s">
@@ -21311,12 +21322,12 @@
       <c r="H22" s="213">
         <v>1</v>
       </c>
-      <c r="I22" s="293">
+      <c r="I22" s="257">
         <v>3</v>
       </c>
-      <c r="J22" s="293"/>
-      <c r="K22" s="293"/>
-      <c r="L22" s="293">
+      <c r="J22" s="257"/>
+      <c r="K22" s="257"/>
+      <c r="L22" s="257">
         <v>6</v>
       </c>
       <c r="M22" s="214" t="s">
@@ -21360,14 +21371,14 @@
       <c r="H23" s="213">
         <v>1</v>
       </c>
-      <c r="I23" s="293">
+      <c r="I23" s="257">
         <v>4</v>
       </c>
-      <c r="J23" s="293"/>
-      <c r="K23" s="293">
+      <c r="J23" s="257"/>
+      <c r="K23" s="257">
         <v>2</v>
       </c>
-      <c r="L23" s="293">
+      <c r="L23" s="257">
         <v>5</v>
       </c>
       <c r="M23" s="214" t="s">
@@ -21415,12 +21426,12 @@
       <c r="H24" s="213">
         <v>1</v>
       </c>
-      <c r="I24" s="293">
+      <c r="I24" s="257">
         <v>1</v>
       </c>
-      <c r="J24" s="293"/>
-      <c r="K24" s="293"/>
-      <c r="L24" s="293">
+      <c r="J24" s="257"/>
+      <c r="K24" s="257"/>
+      <c r="L24" s="257">
         <v>3</v>
       </c>
       <c r="M24" s="214" t="s">
@@ -21478,14 +21489,14 @@
       <c r="H25" s="213">
         <v>1</v>
       </c>
-      <c r="I25" s="293">
+      <c r="I25" s="257">
         <v>6</v>
       </c>
-      <c r="J25" s="293"/>
-      <c r="K25" s="293">
+      <c r="J25" s="257"/>
+      <c r="K25" s="257">
         <v>3</v>
       </c>
-      <c r="L25" s="293">
+      <c r="L25" s="257">
         <v>4</v>
       </c>
       <c r="M25" s="214" t="s">
@@ -21537,10 +21548,10 @@
       <c r="H26" s="213">
         <v>1</v>
       </c>
-      <c r="I26" s="293"/>
-      <c r="J26" s="293"/>
-      <c r="K26" s="293"/>
-      <c r="L26" s="293"/>
+      <c r="I26" s="257"/>
+      <c r="J26" s="257"/>
+      <c r="K26" s="257"/>
+      <c r="L26" s="257"/>
       <c r="M26" s="214" t="s">
         <v>146</v>
       </c>
@@ -21592,10 +21603,10 @@
       <c r="H27" s="213">
         <v>1</v>
       </c>
-      <c r="I27" s="293"/>
-      <c r="J27" s="293"/>
-      <c r="K27" s="293"/>
-      <c r="L27" s="293"/>
+      <c r="I27" s="257"/>
+      <c r="J27" s="257"/>
+      <c r="K27" s="257"/>
+      <c r="L27" s="257"/>
       <c r="M27" s="214" t="s">
         <v>146</v>
       </c>
@@ -21645,10 +21656,10 @@
       <c r="H28" s="213">
         <v>1</v>
       </c>
-      <c r="I28" s="293"/>
-      <c r="J28" s="293"/>
-      <c r="K28" s="293"/>
-      <c r="L28" s="293"/>
+      <c r="I28" s="257"/>
+      <c r="J28" s="257"/>
+      <c r="K28" s="257"/>
+      <c r="L28" s="257"/>
       <c r="M28" s="214" t="s">
         <v>146</v>
       </c>
@@ -21694,10 +21705,10 @@
       <c r="H29" s="213">
         <v>1</v>
       </c>
-      <c r="I29" s="293"/>
-      <c r="J29" s="293"/>
-      <c r="K29" s="293"/>
-      <c r="L29" s="293"/>
+      <c r="I29" s="257"/>
+      <c r="J29" s="257"/>
+      <c r="K29" s="257"/>
+      <c r="L29" s="257"/>
       <c r="M29" s="214" t="s">
         <v>146</v>
       </c>
@@ -21751,10 +21762,10 @@
       <c r="H30" s="225">
         <v>1</v>
       </c>
-      <c r="I30" s="295"/>
-      <c r="J30" s="295"/>
-      <c r="K30" s="295"/>
-      <c r="L30" s="295"/>
+      <c r="I30" s="259"/>
+      <c r="J30" s="259"/>
+      <c r="K30" s="259"/>
+      <c r="L30" s="259"/>
       <c r="M30" s="226" t="s">
         <v>146</v>
       </c>
@@ -21790,10 +21801,10 @@
       <c r="H31" s="213">
         <v>1</v>
       </c>
-      <c r="I31" s="293"/>
-      <c r="J31" s="293"/>
-      <c r="K31" s="293"/>
-      <c r="L31" s="293"/>
+      <c r="I31" s="257"/>
+      <c r="J31" s="257"/>
+      <c r="K31" s="257"/>
+      <c r="L31" s="257"/>
       <c r="M31" s="214" t="s">
         <v>146</v>
       </c>
@@ -21829,10 +21840,10 @@
       <c r="H32" s="213">
         <v>1</v>
       </c>
-      <c r="I32" s="293"/>
-      <c r="J32" s="293"/>
-      <c r="K32" s="293"/>
-      <c r="L32" s="293"/>
+      <c r="I32" s="257"/>
+      <c r="J32" s="257"/>
+      <c r="K32" s="257"/>
+      <c r="L32" s="257"/>
       <c r="M32" s="214" t="s">
         <v>146</v>
       </c>
@@ -21870,10 +21881,10 @@
       <c r="H33" s="225">
         <v>1</v>
       </c>
-      <c r="I33" s="295"/>
-      <c r="J33" s="295"/>
-      <c r="K33" s="295"/>
-      <c r="L33" s="295"/>
+      <c r="I33" s="259"/>
+      <c r="J33" s="259"/>
+      <c r="K33" s="259"/>
+      <c r="L33" s="259"/>
       <c r="M33" s="226" t="s">
         <v>146</v>
       </c>
@@ -21939,10 +21950,10 @@
       <c r="H34" s="231">
         <v>1</v>
       </c>
-      <c r="I34" s="296"/>
-      <c r="J34" s="296"/>
-      <c r="K34" s="296"/>
-      <c r="L34" s="296"/>
+      <c r="I34" s="260"/>
+      <c r="J34" s="260"/>
+      <c r="K34" s="260"/>
+      <c r="L34" s="260"/>
       <c r="M34" s="214" t="s">
         <v>137</v>
       </c>
@@ -21980,10 +21991,10 @@
       <c r="H35" s="213">
         <v>1</v>
       </c>
-      <c r="I35" s="293"/>
-      <c r="J35" s="293"/>
-      <c r="K35" s="293"/>
-      <c r="L35" s="293"/>
+      <c r="I35" s="257"/>
+      <c r="J35" s="257"/>
+      <c r="K35" s="257"/>
+      <c r="L35" s="257"/>
       <c r="M35" s="214" t="s">
         <v>117</v>
       </c>
@@ -22035,10 +22046,10 @@
       <c r="H36" s="213">
         <v>1</v>
       </c>
-      <c r="I36" s="293"/>
-      <c r="J36" s="293"/>
-      <c r="K36" s="293"/>
-      <c r="L36" s="293"/>
+      <c r="I36" s="257"/>
+      <c r="J36" s="257"/>
+      <c r="K36" s="257"/>
+      <c r="L36" s="257"/>
       <c r="M36" s="214"/>
       <c r="N36" s="212"/>
       <c r="O36" s="212"/>
@@ -22072,10 +22083,10 @@
       <c r="H37" s="213">
         <v>1</v>
       </c>
-      <c r="I37" s="293"/>
-      <c r="J37" s="293"/>
-      <c r="K37" s="293"/>
-      <c r="L37" s="293"/>
+      <c r="I37" s="257"/>
+      <c r="J37" s="257"/>
+      <c r="K37" s="257"/>
+      <c r="L37" s="257"/>
       <c r="M37" s="214"/>
       <c r="N37" s="212"/>
       <c r="O37" s="212"/>
@@ -22109,10 +22120,10 @@
       <c r="H38" s="213">
         <v>1</v>
       </c>
-      <c r="I38" s="293"/>
-      <c r="J38" s="293"/>
-      <c r="K38" s="293"/>
-      <c r="L38" s="293"/>
+      <c r="I38" s="257"/>
+      <c r="J38" s="257"/>
+      <c r="K38" s="257"/>
+      <c r="L38" s="257"/>
       <c r="M38" s="214"/>
       <c r="N38" s="212"/>
       <c r="O38" s="212"/>
@@ -22140,10 +22151,10 @@
       <c r="F39" s="234"/>
       <c r="G39" s="196"/>
       <c r="H39" s="235"/>
-      <c r="I39" s="297"/>
-      <c r="J39" s="297"/>
-      <c r="K39" s="297"/>
-      <c r="L39" s="297"/>
+      <c r="I39" s="261"/>
+      <c r="J39" s="261"/>
+      <c r="K39" s="261"/>
+      <c r="L39" s="261"/>
       <c r="M39" s="236"/>
       <c r="N39" s="237"/>
       <c r="O39" s="237"/>
@@ -22198,10 +22209,10 @@
       <c r="F40" s="111"/>
       <c r="G40" s="111"/>
       <c r="H40" s="139"/>
-      <c r="I40" s="291"/>
-      <c r="J40" s="291"/>
-      <c r="K40" s="291"/>
-      <c r="L40" s="291"/>
+      <c r="I40" s="255"/>
+      <c r="J40" s="255"/>
+      <c r="K40" s="255"/>
+      <c r="L40" s="255"/>
       <c r="M40" s="130"/>
       <c r="N40" s="111"/>
       <c r="O40" s="111"/>
@@ -22262,10 +22273,10 @@
         <v>194</v>
       </c>
       <c r="H41" s="189"/>
-      <c r="I41" s="298"/>
-      <c r="J41" s="298"/>
-      <c r="K41" s="298"/>
-      <c r="L41" s="298"/>
+      <c r="I41" s="262"/>
+      <c r="J41" s="262"/>
+      <c r="K41" s="262"/>
+      <c r="L41" s="262"/>
       <c r="M41" s="190" t="s">
         <v>195</v>
       </c>
@@ -22318,10 +22329,10 @@
       <c r="H42" s="194" t="s">
         <v>199</v>
       </c>
-      <c r="I42" s="299"/>
-      <c r="J42" s="299"/>
-      <c r="K42" s="299"/>
-      <c r="L42" s="299"/>
+      <c r="I42" s="263"/>
+      <c r="J42" s="263"/>
+      <c r="K42" s="263"/>
+      <c r="L42" s="263"/>
       <c r="M42" s="175"/>
       <c r="N42" s="155"/>
       <c r="O42" s="155"/>
@@ -22357,10 +22368,10 @@
       <c r="H43" s="213">
         <v>2</v>
       </c>
-      <c r="I43" s="293"/>
-      <c r="J43" s="293"/>
-      <c r="K43" s="293"/>
-      <c r="L43" s="293"/>
+      <c r="I43" s="257"/>
+      <c r="J43" s="257"/>
+      <c r="K43" s="257"/>
+      <c r="L43" s="257"/>
       <c r="M43" s="214" t="s">
         <v>202</v>
       </c>
@@ -22416,10 +22427,10 @@
       <c r="H44" s="213">
         <v>4</v>
       </c>
-      <c r="I44" s="293"/>
-      <c r="J44" s="293"/>
-      <c r="K44" s="293"/>
-      <c r="L44" s="293"/>
+      <c r="I44" s="257"/>
+      <c r="J44" s="257"/>
+      <c r="K44" s="257"/>
+      <c r="L44" s="257"/>
       <c r="M44" s="214" t="s">
         <v>212</v>
       </c>
@@ -22477,10 +22488,10 @@
       <c r="H45" s="213">
         <v>2</v>
       </c>
-      <c r="I45" s="293"/>
-      <c r="J45" s="293"/>
-      <c r="K45" s="293"/>
-      <c r="L45" s="293"/>
+      <c r="I45" s="257"/>
+      <c r="J45" s="257"/>
+      <c r="K45" s="257"/>
+      <c r="L45" s="257"/>
       <c r="M45" s="214" t="s">
         <v>130</v>
       </c>
@@ -22532,10 +22543,10 @@
       <c r="H46" s="213">
         <v>4</v>
       </c>
-      <c r="I46" s="293"/>
-      <c r="J46" s="293"/>
-      <c r="K46" s="293"/>
-      <c r="L46" s="293"/>
+      <c r="I46" s="257"/>
+      <c r="J46" s="257"/>
+      <c r="K46" s="257"/>
+      <c r="L46" s="257"/>
       <c r="M46" s="214" t="s">
         <v>130</v>
       </c>
@@ -22575,10 +22586,10 @@
       <c r="H47" s="213">
         <v>2</v>
       </c>
-      <c r="I47" s="293"/>
-      <c r="J47" s="293"/>
-      <c r="K47" s="293"/>
-      <c r="L47" s="293"/>
+      <c r="I47" s="257"/>
+      <c r="J47" s="257"/>
+      <c r="K47" s="257"/>
+      <c r="L47" s="257"/>
       <c r="M47" s="214" t="s">
         <v>146</v>
       </c>
@@ -22618,10 +22629,10 @@
       <c r="H48" s="213">
         <v>4</v>
       </c>
-      <c r="I48" s="293"/>
-      <c r="J48" s="293"/>
-      <c r="K48" s="293"/>
-      <c r="L48" s="293"/>
+      <c r="I48" s="257"/>
+      <c r="J48" s="257"/>
+      <c r="K48" s="257"/>
+      <c r="L48" s="257"/>
       <c r="M48" s="214" t="s">
         <v>117</v>
       </c>
@@ -22677,10 +22688,10 @@
       <c r="H49" s="220">
         <v>2</v>
       </c>
-      <c r="I49" s="294"/>
-      <c r="J49" s="294"/>
-      <c r="K49" s="294"/>
-      <c r="L49" s="294"/>
+      <c r="I49" s="258"/>
+      <c r="J49" s="258"/>
+      <c r="K49" s="258"/>
+      <c r="L49" s="258"/>
       <c r="M49" s="221" t="s">
         <v>223</v>
       </c>
@@ -22766,10 +22777,10 @@
       <c r="H50" s="213">
         <v>4</v>
       </c>
-      <c r="I50" s="293"/>
-      <c r="J50" s="293"/>
-      <c r="K50" s="293"/>
-      <c r="L50" s="293"/>
+      <c r="I50" s="257"/>
+      <c r="J50" s="257"/>
+      <c r="K50" s="257"/>
+      <c r="L50" s="257"/>
       <c r="M50" s="214" t="s">
         <v>223</v>
       </c>
@@ -22815,12 +22826,12 @@
       <c r="H51" s="213">
         <v>2</v>
       </c>
-      <c r="I51" s="293"/>
-      <c r="J51" s="293"/>
-      <c r="K51" s="293">
+      <c r="I51" s="257"/>
+      <c r="J51" s="257"/>
+      <c r="K51" s="257">
         <v>6</v>
       </c>
-      <c r="L51" s="293">
+      <c r="L51" s="257">
         <v>4</v>
       </c>
       <c r="M51" s="214" t="s">
@@ -22872,12 +22883,12 @@
       <c r="H52" s="213">
         <v>4</v>
       </c>
-      <c r="I52" s="293"/>
-      <c r="J52" s="293"/>
-      <c r="K52" s="293">
+      <c r="I52" s="257"/>
+      <c r="J52" s="257"/>
+      <c r="K52" s="257">
         <v>1</v>
       </c>
-      <c r="L52" s="293"/>
+      <c r="L52" s="257"/>
       <c r="M52" s="214" t="s">
         <v>223</v>
       </c>
@@ -22919,10 +22930,10 @@
       <c r="H53" s="213">
         <v>2</v>
       </c>
-      <c r="I53" s="293"/>
-      <c r="J53" s="293"/>
-      <c r="K53" s="293"/>
-      <c r="L53" s="293"/>
+      <c r="I53" s="257"/>
+      <c r="J53" s="257"/>
+      <c r="K53" s="257"/>
+      <c r="L53" s="257"/>
       <c r="M53" s="214" t="s">
         <v>236</v>
       </c>
@@ -22964,10 +22975,10 @@
       <c r="H54" s="213">
         <v>4</v>
       </c>
-      <c r="I54" s="293"/>
-      <c r="J54" s="293"/>
-      <c r="K54" s="293"/>
-      <c r="L54" s="293">
+      <c r="I54" s="257"/>
+      <c r="J54" s="257"/>
+      <c r="K54" s="257"/>
+      <c r="L54" s="257">
         <v>3</v>
       </c>
       <c r="M54" s="214" t="s">
@@ -23013,12 +23024,12 @@
       <c r="H55" s="213">
         <v>2</v>
       </c>
-      <c r="I55" s="293"/>
-      <c r="J55" s="293"/>
-      <c r="K55" s="293">
+      <c r="I55" s="257"/>
+      <c r="J55" s="257"/>
+      <c r="K55" s="257">
         <v>4</v>
       </c>
-      <c r="L55" s="293"/>
+      <c r="L55" s="257"/>
       <c r="M55" s="214" t="s">
         <v>236</v>
       </c>
@@ -23072,12 +23083,12 @@
       <c r="H56" s="213">
         <v>4</v>
       </c>
-      <c r="I56" s="293"/>
-      <c r="J56" s="293">
+      <c r="I56" s="257"/>
+      <c r="J56" s="257">
         <v>1</v>
       </c>
-      <c r="K56" s="293"/>
-      <c r="L56" s="293">
+      <c r="K56" s="257"/>
+      <c r="L56" s="257">
         <v>6</v>
       </c>
       <c r="M56" s="214" t="s">
@@ -23131,12 +23142,12 @@
       <c r="H57" s="213">
         <v>2</v>
       </c>
-      <c r="I57" s="293"/>
-      <c r="J57" s="293">
+      <c r="I57" s="257"/>
+      <c r="J57" s="257">
         <v>4</v>
       </c>
-      <c r="K57" s="293"/>
-      <c r="L57" s="293">
+      <c r="K57" s="257"/>
+      <c r="L57" s="257">
         <v>2</v>
       </c>
       <c r="M57" s="214" t="s">
@@ -23186,12 +23197,12 @@
       <c r="H58" s="213">
         <v>4</v>
       </c>
-      <c r="I58" s="293"/>
-      <c r="J58" s="293">
+      <c r="I58" s="257"/>
+      <c r="J58" s="257">
         <v>2</v>
       </c>
-      <c r="K58" s="293"/>
-      <c r="L58" s="293">
+      <c r="K58" s="257"/>
+      <c r="L58" s="257">
         <v>5</v>
       </c>
       <c r="M58" s="214" t="s">
@@ -23239,12 +23250,12 @@
       <c r="H59" s="213">
         <v>2</v>
       </c>
-      <c r="I59" s="293"/>
-      <c r="J59" s="293">
+      <c r="I59" s="257"/>
+      <c r="J59" s="257">
         <v>3</v>
       </c>
-      <c r="K59" s="293"/>
-      <c r="L59" s="293"/>
+      <c r="K59" s="257"/>
+      <c r="L59" s="257"/>
       <c r="M59" s="214" t="s">
         <v>236</v>
       </c>
@@ -23288,12 +23299,12 @@
       <c r="H60" s="213">
         <v>4</v>
       </c>
-      <c r="I60" s="293"/>
-      <c r="J60" s="293">
+      <c r="I60" s="257"/>
+      <c r="J60" s="257">
         <v>5</v>
       </c>
-      <c r="K60" s="293"/>
-      <c r="L60" s="293"/>
+      <c r="K60" s="257"/>
+      <c r="L60" s="257"/>
       <c r="M60" s="214" t="s">
         <v>236</v>
       </c>
@@ -23347,12 +23358,12 @@
       <c r="H61" s="225">
         <v>2</v>
       </c>
-      <c r="I61" s="295"/>
-      <c r="J61" s="295">
+      <c r="I61" s="259"/>
+      <c r="J61" s="259">
         <v>6</v>
       </c>
-      <c r="K61" s="295"/>
-      <c r="L61" s="295">
+      <c r="K61" s="259"/>
+      <c r="L61" s="259">
         <v>1</v>
       </c>
       <c r="M61" s="226" t="s">
@@ -23390,10 +23401,10 @@
       <c r="H62" s="213">
         <v>4</v>
       </c>
-      <c r="I62" s="293"/>
-      <c r="J62" s="293"/>
-      <c r="K62" s="293"/>
-      <c r="L62" s="293"/>
+      <c r="I62" s="257"/>
+      <c r="J62" s="257"/>
+      <c r="K62" s="257"/>
+      <c r="L62" s="257"/>
       <c r="M62" s="214" t="s">
         <v>236</v>
       </c>
@@ -23429,10 +23440,10 @@
       <c r="H63" s="213">
         <v>2</v>
       </c>
-      <c r="I63" s="293"/>
-      <c r="J63" s="293"/>
-      <c r="K63" s="293"/>
-      <c r="L63" s="293"/>
+      <c r="I63" s="257"/>
+      <c r="J63" s="257"/>
+      <c r="K63" s="257"/>
+      <c r="L63" s="257"/>
       <c r="M63" s="214" t="s">
         <v>236</v>
       </c>
@@ -23468,10 +23479,10 @@
       <c r="H64" s="225">
         <v>4</v>
       </c>
-      <c r="I64" s="295"/>
-      <c r="J64" s="295"/>
-      <c r="K64" s="295"/>
-      <c r="L64" s="295"/>
+      <c r="I64" s="259"/>
+      <c r="J64" s="259"/>
+      <c r="K64" s="259"/>
+      <c r="L64" s="259"/>
       <c r="M64" s="226" t="s">
         <v>236</v>
       </c>
@@ -23539,10 +23550,10 @@
       <c r="H65" s="213">
         <v>2</v>
       </c>
-      <c r="I65" s="293"/>
-      <c r="J65" s="293"/>
-      <c r="K65" s="293"/>
-      <c r="L65" s="293"/>
+      <c r="I65" s="257"/>
+      <c r="J65" s="257"/>
+      <c r="K65" s="257"/>
+      <c r="L65" s="257"/>
       <c r="M65" s="214" t="s">
         <v>137</v>
       </c>
@@ -23578,10 +23589,10 @@
       <c r="H66" s="213">
         <v>4</v>
       </c>
-      <c r="I66" s="293"/>
-      <c r="J66" s="293"/>
-      <c r="K66" s="293"/>
-      <c r="L66" s="293"/>
+      <c r="I66" s="257"/>
+      <c r="J66" s="257"/>
+      <c r="K66" s="257"/>
+      <c r="L66" s="257"/>
       <c r="M66" s="214"/>
       <c r="N66" s="212"/>
       <c r="O66" s="212"/>
@@ -23618,10 +23629,10 @@
       <c r="H67" s="213">
         <v>2</v>
       </c>
-      <c r="I67" s="293"/>
-      <c r="J67" s="293"/>
-      <c r="K67" s="293"/>
-      <c r="L67" s="293"/>
+      <c r="I67" s="257"/>
+      <c r="J67" s="257"/>
+      <c r="K67" s="257"/>
+      <c r="L67" s="257"/>
       <c r="M67" s="214"/>
       <c r="N67" s="212"/>
       <c r="O67" s="212"/>
@@ -23655,10 +23666,10 @@
       <c r="H68" s="213">
         <v>4</v>
       </c>
-      <c r="I68" s="293"/>
-      <c r="J68" s="293"/>
-      <c r="K68" s="293"/>
-      <c r="L68" s="293"/>
+      <c r="I68" s="257"/>
+      <c r="J68" s="257"/>
+      <c r="K68" s="257"/>
+      <c r="L68" s="257"/>
       <c r="M68" s="214"/>
       <c r="N68" s="212"/>
       <c r="O68" s="212"/>
@@ -23692,10 +23703,10 @@
       <c r="H69" s="213">
         <v>2</v>
       </c>
-      <c r="I69" s="293"/>
-      <c r="J69" s="293"/>
-      <c r="K69" s="293"/>
-      <c r="L69" s="293"/>
+      <c r="I69" s="257"/>
+      <c r="J69" s="257"/>
+      <c r="K69" s="257"/>
+      <c r="L69" s="257"/>
       <c r="M69" s="214"/>
       <c r="N69" s="212"/>
       <c r="O69" s="212"/>
@@ -23753,10 +23764,10 @@
       <c r="F70" s="239"/>
       <c r="G70" s="199"/>
       <c r="H70" s="213"/>
-      <c r="I70" s="293"/>
-      <c r="J70" s="293"/>
-      <c r="K70" s="293"/>
-      <c r="L70" s="293"/>
+      <c r="I70" s="257"/>
+      <c r="J70" s="257"/>
+      <c r="K70" s="257"/>
+      <c r="L70" s="257"/>
       <c r="M70" s="214"/>
       <c r="N70" s="212"/>
       <c r="O70" s="212"/>
@@ -23811,10 +23822,10 @@
       <c r="F71" s="111"/>
       <c r="G71" s="111"/>
       <c r="H71" s="139"/>
-      <c r="I71" s="291"/>
-      <c r="J71" s="291"/>
-      <c r="K71" s="291"/>
-      <c r="L71" s="291"/>
+      <c r="I71" s="255"/>
+      <c r="J71" s="255"/>
+      <c r="K71" s="255"/>
+      <c r="L71" s="255"/>
       <c r="M71" s="130"/>
       <c r="N71" s="111"/>
       <c r="O71" s="111"/>
@@ -23875,10 +23886,10 @@
         <v>194</v>
       </c>
       <c r="H72" s="144"/>
-      <c r="I72" s="300"/>
-      <c r="J72" s="300"/>
-      <c r="K72" s="300"/>
-      <c r="L72" s="300"/>
+      <c r="I72" s="264"/>
+      <c r="J72" s="264"/>
+      <c r="K72" s="264"/>
+      <c r="L72" s="264"/>
       <c r="M72" s="156" t="s">
         <v>195</v>
       </c>
@@ -23961,10 +23972,10 @@
       <c r="H73" s="135" t="s">
         <v>199</v>
       </c>
-      <c r="I73" s="290"/>
-      <c r="J73" s="290"/>
-      <c r="K73" s="290"/>
-      <c r="L73" s="290"/>
+      <c r="I73" s="254"/>
+      <c r="J73" s="254"/>
+      <c r="K73" s="254"/>
+      <c r="L73" s="254"/>
       <c r="M73" s="150"/>
       <c r="N73" s="127"/>
       <c r="O73" s="127"/>
@@ -24030,10 +24041,10 @@
       <c r="H74" s="213">
         <v>3</v>
       </c>
-      <c r="I74" s="293"/>
-      <c r="J74" s="293"/>
-      <c r="K74" s="293"/>
-      <c r="L74" s="293"/>
+      <c r="I74" s="257"/>
+      <c r="J74" s="257"/>
+      <c r="K74" s="257"/>
+      <c r="L74" s="257"/>
       <c r="M74" s="214" t="s">
         <v>115</v>
       </c>
@@ -24089,10 +24100,10 @@
       <c r="H75" s="213">
         <v>5</v>
       </c>
-      <c r="I75" s="293"/>
-      <c r="J75" s="293"/>
-      <c r="K75" s="293"/>
-      <c r="L75" s="293"/>
+      <c r="I75" s="257"/>
+      <c r="J75" s="257"/>
+      <c r="K75" s="257"/>
+      <c r="L75" s="257"/>
       <c r="M75" s="214" t="s">
         <v>115</v>
       </c>
@@ -24136,10 +24147,10 @@
       <c r="H76" s="213">
         <v>3</v>
       </c>
-      <c r="I76" s="293"/>
-      <c r="J76" s="293"/>
-      <c r="K76" s="293"/>
-      <c r="L76" s="293"/>
+      <c r="I76" s="257"/>
+      <c r="J76" s="257"/>
+      <c r="K76" s="257"/>
+      <c r="L76" s="257"/>
       <c r="M76" s="214" t="s">
         <v>115</v>
       </c>
@@ -24187,10 +24198,10 @@
       <c r="H77" s="213">
         <v>5</v>
       </c>
-      <c r="I77" s="293"/>
-      <c r="J77" s="293"/>
-      <c r="K77" s="293"/>
-      <c r="L77" s="293"/>
+      <c r="I77" s="257"/>
+      <c r="J77" s="257"/>
+      <c r="K77" s="257"/>
+      <c r="L77" s="257"/>
       <c r="M77" s="214" t="s">
         <v>115</v>
       </c>
@@ -24238,10 +24249,10 @@
       <c r="H78" s="213">
         <v>3</v>
       </c>
-      <c r="I78" s="293"/>
-      <c r="J78" s="293"/>
-      <c r="K78" s="293"/>
-      <c r="L78" s="293"/>
+      <c r="I78" s="257"/>
+      <c r="J78" s="257"/>
+      <c r="K78" s="257"/>
+      <c r="L78" s="257"/>
       <c r="M78" s="214" t="s">
         <v>115</v>
       </c>
@@ -24287,10 +24298,10 @@
       <c r="H79" s="213">
         <v>5</v>
       </c>
-      <c r="I79" s="293"/>
-      <c r="J79" s="293"/>
-      <c r="K79" s="293"/>
-      <c r="L79" s="293"/>
+      <c r="I79" s="257"/>
+      <c r="J79" s="257"/>
+      <c r="K79" s="257"/>
+      <c r="L79" s="257"/>
       <c r="M79" s="214" t="s">
         <v>117</v>
       </c>
@@ -24344,10 +24355,10 @@
       <c r="H80" s="220">
         <v>3</v>
       </c>
-      <c r="I80" s="294"/>
-      <c r="J80" s="294"/>
-      <c r="K80" s="294"/>
-      <c r="L80" s="294"/>
+      <c r="I80" s="258"/>
+      <c r="J80" s="258"/>
+      <c r="K80" s="258"/>
+      <c r="L80" s="258"/>
       <c r="M80" s="221" t="s">
         <v>115</v>
       </c>
@@ -24427,10 +24438,10 @@
       <c r="H81" s="213">
         <v>5</v>
       </c>
-      <c r="I81" s="293"/>
-      <c r="J81" s="293"/>
-      <c r="K81" s="293"/>
-      <c r="L81" s="293"/>
+      <c r="I81" s="257"/>
+      <c r="J81" s="257"/>
+      <c r="K81" s="257"/>
+      <c r="L81" s="257"/>
       <c r="M81" s="214" t="s">
         <v>115</v>
       </c>
@@ -24476,10 +24487,10 @@
       <c r="H82" s="213">
         <v>3</v>
       </c>
-      <c r="I82" s="293"/>
-      <c r="J82" s="293"/>
-      <c r="K82" s="293"/>
-      <c r="L82" s="293"/>
+      <c r="I82" s="257"/>
+      <c r="J82" s="257"/>
+      <c r="K82" s="257"/>
+      <c r="L82" s="257"/>
       <c r="M82" s="214" t="s">
         <v>115</v>
       </c>
@@ -24533,10 +24544,10 @@
       <c r="H83" s="213">
         <v>5</v>
       </c>
-      <c r="I83" s="293"/>
-      <c r="J83" s="293"/>
-      <c r="K83" s="293"/>
-      <c r="L83" s="293"/>
+      <c r="I83" s="257"/>
+      <c r="J83" s="257"/>
+      <c r="K83" s="257"/>
+      <c r="L83" s="257"/>
       <c r="M83" s="214" t="s">
         <v>115</v>
       </c>
@@ -24584,10 +24595,10 @@
       <c r="H84" s="213">
         <v>3</v>
       </c>
-      <c r="I84" s="293"/>
-      <c r="J84" s="293"/>
-      <c r="K84" s="293"/>
-      <c r="L84" s="293"/>
+      <c r="I84" s="257"/>
+      <c r="J84" s="257"/>
+      <c r="K84" s="257"/>
+      <c r="L84" s="257"/>
       <c r="M84" s="214" t="s">
         <v>115</v>
       </c>
@@ -24627,10 +24638,10 @@
       <c r="H85" s="213">
         <v>5</v>
       </c>
-      <c r="I85" s="293"/>
-      <c r="J85" s="293"/>
-      <c r="K85" s="293"/>
-      <c r="L85" s="293"/>
+      <c r="I85" s="257"/>
+      <c r="J85" s="257"/>
+      <c r="K85" s="257"/>
+      <c r="L85" s="257"/>
       <c r="M85" s="214" t="s">
         <v>115</v>
       </c>
@@ -24678,10 +24689,10 @@
       <c r="H86" s="213">
         <v>3</v>
       </c>
-      <c r="I86" s="293"/>
-      <c r="J86" s="293"/>
-      <c r="K86" s="293"/>
-      <c r="L86" s="293"/>
+      <c r="I86" s="257"/>
+      <c r="J86" s="257"/>
+      <c r="K86" s="257"/>
+      <c r="L86" s="257"/>
       <c r="M86" s="214" t="s">
         <v>115</v>
       </c>
@@ -24729,10 +24740,10 @@
       <c r="H87" s="213">
         <v>5</v>
       </c>
-      <c r="I87" s="293"/>
-      <c r="J87" s="293"/>
-      <c r="K87" s="293"/>
-      <c r="L87" s="293"/>
+      <c r="I87" s="257"/>
+      <c r="J87" s="257"/>
+      <c r="K87" s="257"/>
+      <c r="L87" s="257"/>
       <c r="M87" s="214" t="s">
         <v>311</v>
       </c>
@@ -24792,10 +24803,10 @@
       <c r="H88" s="213">
         <v>3</v>
       </c>
-      <c r="I88" s="293"/>
-      <c r="J88" s="293"/>
-      <c r="K88" s="293"/>
-      <c r="L88" s="293"/>
+      <c r="I88" s="257"/>
+      <c r="J88" s="257"/>
+      <c r="K88" s="257"/>
+      <c r="L88" s="257"/>
       <c r="M88" s="214" t="s">
         <v>314</v>
       </c>
@@ -24835,10 +24846,10 @@
       <c r="H89" s="213">
         <v>5</v>
       </c>
-      <c r="I89" s="293"/>
-      <c r="J89" s="293"/>
-      <c r="K89" s="293"/>
-      <c r="L89" s="293"/>
+      <c r="I89" s="257"/>
+      <c r="J89" s="257"/>
+      <c r="K89" s="257"/>
+      <c r="L89" s="257"/>
       <c r="M89" s="214" t="s">
         <v>317</v>
       </c>
@@ -24896,10 +24907,10 @@
       <c r="H90" s="213">
         <v>3</v>
       </c>
-      <c r="I90" s="293"/>
-      <c r="J90" s="293"/>
-      <c r="K90" s="293"/>
-      <c r="L90" s="293"/>
+      <c r="I90" s="257"/>
+      <c r="J90" s="257"/>
+      <c r="K90" s="257"/>
+      <c r="L90" s="257"/>
       <c r="M90" s="214" t="s">
         <v>319</v>
       </c>
@@ -24955,10 +24966,10 @@
       <c r="H91" s="213">
         <v>5</v>
       </c>
-      <c r="I91" s="293"/>
-      <c r="J91" s="293"/>
-      <c r="K91" s="293"/>
-      <c r="L91" s="293"/>
+      <c r="I91" s="257"/>
+      <c r="J91" s="257"/>
+      <c r="K91" s="257"/>
+      <c r="L91" s="257"/>
       <c r="M91" s="214" t="s">
         <v>115</v>
       </c>
@@ -25010,10 +25021,10 @@
       <c r="H92" s="225">
         <v>3</v>
       </c>
-      <c r="I92" s="295"/>
-      <c r="J92" s="295"/>
-      <c r="K92" s="295"/>
-      <c r="L92" s="295"/>
+      <c r="I92" s="259"/>
+      <c r="J92" s="259"/>
+      <c r="K92" s="259"/>
+      <c r="L92" s="259"/>
       <c r="M92" s="226" t="s">
         <v>115</v>
       </c>
@@ -25049,10 +25060,10 @@
       <c r="H93" s="213">
         <v>5</v>
       </c>
-      <c r="I93" s="293"/>
-      <c r="J93" s="293"/>
-      <c r="K93" s="293"/>
-      <c r="L93" s="293"/>
+      <c r="I93" s="257"/>
+      <c r="J93" s="257"/>
+      <c r="K93" s="257"/>
+      <c r="L93" s="257"/>
       <c r="M93" s="214" t="s">
         <v>115</v>
       </c>
@@ -25088,10 +25099,10 @@
       <c r="H94" s="213">
         <v>3</v>
       </c>
-      <c r="I94" s="293"/>
-      <c r="J94" s="293"/>
-      <c r="K94" s="293"/>
-      <c r="L94" s="293"/>
+      <c r="I94" s="257"/>
+      <c r="J94" s="257"/>
+      <c r="K94" s="257"/>
+      <c r="L94" s="257"/>
       <c r="M94" s="214" t="s">
         <v>115</v>
       </c>
@@ -25127,10 +25138,10 @@
       <c r="H95" s="225">
         <v>5</v>
       </c>
-      <c r="I95" s="295"/>
-      <c r="J95" s="295"/>
-      <c r="K95" s="295"/>
-      <c r="L95" s="295"/>
+      <c r="I95" s="259"/>
+      <c r="J95" s="259"/>
+      <c r="K95" s="259"/>
+      <c r="L95" s="259"/>
       <c r="M95" s="226" t="s">
         <v>115</v>
       </c>
@@ -25198,10 +25209,10 @@
       <c r="H96" s="213">
         <v>3</v>
       </c>
-      <c r="I96" s="293"/>
-      <c r="J96" s="293"/>
-      <c r="K96" s="293"/>
-      <c r="L96" s="293"/>
+      <c r="I96" s="257"/>
+      <c r="J96" s="257"/>
+      <c r="K96" s="257"/>
+      <c r="L96" s="257"/>
       <c r="M96" s="214" t="s">
         <v>137</v>
       </c>
@@ -25239,10 +25250,10 @@
       <c r="H97" s="213">
         <v>5</v>
       </c>
-      <c r="I97" s="293"/>
-      <c r="J97" s="293"/>
-      <c r="K97" s="293"/>
-      <c r="L97" s="293"/>
+      <c r="I97" s="257"/>
+      <c r="J97" s="257"/>
+      <c r="K97" s="257"/>
+      <c r="L97" s="257"/>
       <c r="M97" s="214" t="s">
         <v>137</v>
       </c>
@@ -25280,10 +25291,10 @@
       <c r="H98" s="213">
         <v>3</v>
       </c>
-      <c r="I98" s="293"/>
-      <c r="J98" s="293"/>
-      <c r="K98" s="293"/>
-      <c r="L98" s="293"/>
+      <c r="I98" s="257"/>
+      <c r="J98" s="257"/>
+      <c r="K98" s="257"/>
+      <c r="L98" s="257"/>
       <c r="M98" s="214"/>
       <c r="N98" s="212"/>
       <c r="O98" s="212"/>
@@ -25317,10 +25328,10 @@
       <c r="H99" s="213">
         <v>5</v>
       </c>
-      <c r="I99" s="293"/>
-      <c r="J99" s="293"/>
-      <c r="K99" s="293"/>
-      <c r="L99" s="293"/>
+      <c r="I99" s="257"/>
+      <c r="J99" s="257"/>
+      <c r="K99" s="257"/>
+      <c r="L99" s="257"/>
       <c r="M99" s="214"/>
       <c r="N99" s="212"/>
       <c r="O99" s="212"/>
@@ -25354,10 +25365,10 @@
       <c r="H100" s="213">
         <v>3</v>
       </c>
-      <c r="I100" s="293"/>
-      <c r="J100" s="293"/>
-      <c r="K100" s="293"/>
-      <c r="L100" s="293"/>
+      <c r="I100" s="257"/>
+      <c r="J100" s="257"/>
+      <c r="K100" s="257"/>
+      <c r="L100" s="257"/>
       <c r="M100" s="214"/>
       <c r="N100" s="212"/>
       <c r="O100" s="212"/>
@@ -25391,10 +25402,10 @@
       <c r="H101" s="225">
         <v>5</v>
       </c>
-      <c r="I101" s="295"/>
-      <c r="J101" s="295"/>
-      <c r="K101" s="295"/>
-      <c r="L101" s="295"/>
+      <c r="I101" s="259"/>
+      <c r="J101" s="259"/>
+      <c r="K101" s="259"/>
+      <c r="L101" s="259"/>
       <c r="M101" s="226"/>
       <c r="N101" s="224"/>
       <c r="O101" s="224"/>
@@ -25424,10 +25435,10 @@
         <v>117</v>
       </c>
       <c r="H102" s="249"/>
-      <c r="I102" s="301"/>
-      <c r="J102" s="301"/>
-      <c r="K102" s="301"/>
-      <c r="L102" s="301"/>
+      <c r="I102" s="265"/>
+      <c r="J102" s="265"/>
+      <c r="K102" s="265"/>
+      <c r="L102" s="265"/>
       <c r="M102" s="250"/>
       <c r="N102" s="251"/>
       <c r="O102" s="251"/>
@@ -26478,9 +26489,9 @@
       <c r="T3" s="103" t="s">
         <v>329</v>
       </c>
-      <c r="U3">
+      <c r="U3" t="e">
         <f>MATCH(T2,WatchBillColumns,0)</f>
-        <v>21</v>
+        <v>#N/A</v>
       </c>
       <c r="W3" s="103" t="s">
         <v>329</v>
@@ -26587,7 +26598,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">IF(AND(COUNTIF(T6:T55,"&lt;&gt; ")=COUNTIF(U6:U55,"&lt;&gt;"),COUNTIF(U6:U55,"&lt;&gt;")=COUNTIF(V6:V55,"&lt;&gt;*E*")),"Yes","No")</f>
-        <v>Yes</v>
+        <v>No</v>
       </c>
       <c r="W4" s="103" t="s">
         <v>330</v>
@@ -26807,14 +26818,14 @@
       </c>
       <c r="T6" t="str">
         <f t="array" aca="1" ref="T6" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(1:1)))," ")</f>
-        <v>OIC</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U6" t="s">
         <v>116</v>
       </c>
       <c r="V6" t="str">
         <f t="array" aca="1" ref="V6" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T6,COUNTIF(T$6:T$55,T6)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U6,COUNTIF(U$6:U$55,U6)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>1-1</v>
+        <v>E-E</v>
       </c>
       <c r="W6" t="str">
         <f t="array" aca="1" ref="W6" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(1:1)))," ")</f>
@@ -26886,7 +26897,7 @@
         <f t="array" aca="1" ref="AO6" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(1:1)))," ")</f>
         <v>5</v>
       </c>
-      <c r="AP6" s="302">
+      <c r="AP6" s="266">
         <v>1</v>
       </c>
       <c r="AQ6" t="str">
@@ -26897,7 +26908,7 @@
         <f t="array" aca="1" ref="AR6" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(1:1)))," ")</f>
         <v>1</v>
       </c>
-      <c r="AS6" s="302">
+      <c r="AS6" s="266">
         <v>1</v>
       </c>
       <c r="AT6" t="str">
@@ -26974,14 +26985,14 @@
       </c>
       <c r="T7" t="str">
         <f t="array" aca="1" ref="T7" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(2:2)))," ")</f>
-        <v>Fix/Radio</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U7" t="s">
         <v>123</v>
       </c>
       <c r="V7" t="str">
         <f t="array" aca="1" ref="V7" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T7,COUNTIF(T$6:T$55,T7)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U7,COUNTIF(U$6:U$55,U7)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>2-2</v>
+        <v>E-E</v>
       </c>
       <c r="W7" t="str">
         <f t="array" aca="1" ref="W7" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(2:2)))," ")</f>
@@ -27053,7 +27064,7 @@
         <f t="array" aca="1" ref="AO7" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(2:2)))," ")</f>
         <v>2</v>
       </c>
-      <c r="AP7" s="302">
+      <c r="AP7" s="266">
         <v>2</v>
       </c>
       <c r="AQ7" t="str">
@@ -27064,7 +27075,7 @@
         <f t="array" aca="1" ref="AR7" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(2:2)))," ")</f>
         <v>2</v>
       </c>
-      <c r="AS7" s="302">
+      <c r="AS7" s="266">
         <v>2</v>
       </c>
       <c r="AT7" t="str">
@@ -27141,14 +27152,14 @@
       </c>
       <c r="T8" t="str">
         <f t="array" aca="1" ref="T8" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(3:3)))," ")</f>
-        <v>ER Elec.Brd./Pumps</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U8" t="s">
         <v>131</v>
       </c>
       <c r="V8" t="str">
         <f t="array" aca="1" ref="V8" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T8,COUNTIF(T$6:T$55,T8)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U8,COUNTIF(U$6:U$55,U8)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>3-3</v>
+        <v>E-E</v>
       </c>
       <c r="W8" t="str">
         <f t="array" aca="1" ref="W8" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(3:3)))," ")</f>
@@ -27220,7 +27231,7 @@
         <f t="array" aca="1" ref="AO8" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(3:3)))," ")</f>
         <v>3</v>
       </c>
-      <c r="AP8" s="302">
+      <c r="AP8" s="266">
         <v>3</v>
       </c>
       <c r="AQ8" t="str">
@@ -27231,7 +27242,7 @@
         <f t="array" aca="1" ref="AR8" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(3:3)))," ")</f>
         <v>6</v>
       </c>
-      <c r="AS8" s="302">
+      <c r="AS8" s="266">
         <v>3</v>
       </c>
       <c r="AT8" t="str">
@@ -27308,14 +27319,14 @@
       </c>
       <c r="T9" t="str">
         <f t="array" aca="1" ref="T9" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(4:4)))," ")</f>
-        <v>DC Party</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U9" t="s">
         <v>134</v>
       </c>
       <c r="V9" t="str">
         <f t="array" aca="1" ref="V9" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T9,COUNTIF(T$6:T$55,T9)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U9,COUNTIF(U$6:U$55,U9)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>4-4</v>
+        <v>E-E</v>
       </c>
       <c r="W9" t="str">
         <f t="array" aca="1" ref="W9" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(4:4)))," ")</f>
@@ -27387,7 +27398,7 @@
         <f t="array" aca="1" ref="AO9" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(4:4)))," ")</f>
         <v>6</v>
       </c>
-      <c r="AP9" s="302">
+      <c r="AP9" s="266">
         <v>4</v>
       </c>
       <c r="AQ9" t="str">
@@ -27398,7 +27409,7 @@
         <f t="array" aca="1" ref="AR9" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(4:4)))," ")</f>
         <v>5</v>
       </c>
-      <c r="AS9" s="302">
+      <c r="AS9" s="266">
         <v>4</v>
       </c>
       <c r="AT9" t="str">
@@ -27475,14 +27486,14 @@
       </c>
       <c r="T10" t="str">
         <f t="array" aca="1" ref="T10" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(5:5)))," ")</f>
-        <v>HDCT</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U10" t="s">
         <v>149</v>
       </c>
       <c r="V10" t="str">
         <f t="array" aca="1" ref="V10" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T10,COUNTIF(T$6:T$55,T10)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U10,COUNTIF(U$6:U$55,U10)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>5-5</v>
+        <v>E-E</v>
       </c>
       <c r="W10" t="str">
         <f t="array" aca="1" ref="W10" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(5:5)))," ")</f>
@@ -27554,7 +27565,7 @@
         <f t="array" aca="1" ref="AO10" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(5:5)))," ")</f>
         <v>1</v>
       </c>
-      <c r="AP10" s="302">
+      <c r="AP10" s="266">
         <v>5</v>
       </c>
       <c r="AQ10" t="str">
@@ -27565,7 +27576,7 @@
         <f t="array" aca="1" ref="AR10" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(5:5)))," ")</f>
         <v>3</v>
       </c>
-      <c r="AS10" s="302">
+      <c r="AS10" s="266">
         <v>5</v>
       </c>
       <c r="AT10" t="str">
@@ -27642,14 +27653,14 @@
       </c>
       <c r="T11" t="str">
         <f t="array" aca="1" ref="T11" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(6:6)))," ")</f>
-        <v>DC Party</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U11" t="s">
         <v>134</v>
       </c>
       <c r="V11" t="str">
         <f t="array" aca="1" ref="V11" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T11,COUNTIF(T$6:T$55,T11)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U11,COUNTIF(U$6:U$55,U11)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>4-4</v>
+        <v>E-E</v>
       </c>
       <c r="W11" t="str">
         <f t="array" aca="1" ref="W11" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(6:6)))," ")</f>
@@ -27721,7 +27732,7 @@
         <f t="array" aca="1" ref="AO11" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AP$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(6:6)))," ")</f>
         <v>4</v>
       </c>
-      <c r="AP11" s="302">
+      <c r="AP11" s="266">
         <v>6</v>
       </c>
       <c r="AQ11" t="str">
@@ -27732,7 +27743,7 @@
         <f t="array" aca="1" ref="AR11" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(6:6)))," ")</f>
         <v>4</v>
       </c>
-      <c r="AS11" s="302">
+      <c r="AS11" s="266">
         <v>6</v>
       </c>
       <c r="AT11" t="str">
@@ -27809,14 +27820,14 @@
       </c>
       <c r="T12" t="str">
         <f t="array" aca="1" ref="T12" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(7:7)))," ")</f>
-        <v>Damage Control</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U12" t="s">
         <v>196</v>
       </c>
       <c r="V12" t="str">
         <f t="array" aca="1" ref="V12" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T12,COUNTIF(T$6:T$55,T12)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U12,COUNTIF(U$6:U$55,U12)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>7-7</v>
+        <v>E-E</v>
       </c>
       <c r="W12" t="str">
         <f t="array" aca="1" ref="W12" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(7:7)))," ")</f>
@@ -27890,7 +27901,7 @@
         <f t="array" aca="1" ref="AR12" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(7:7)))," ")</f>
         <v>4</v>
       </c>
-      <c r="AS12" s="302">
+      <c r="AS12" s="266">
         <v>1</v>
       </c>
       <c r="AT12" t="str">
@@ -27967,14 +27978,14 @@
       </c>
       <c r="T13" t="str">
         <f t="array" aca="1" ref="T13" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(8:8)))," ")</f>
-        <v>Officer I/C DC</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U13" t="s">
         <v>207</v>
       </c>
       <c r="V13" t="str">
         <f t="array" aca="1" ref="V13" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T13,COUNTIF(T$6:T$55,T13)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U13,COUNTIF(U$6:U$55,U13)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>8-8</v>
+        <v>E-E</v>
       </c>
       <c r="W13" t="str">
         <f t="array" aca="1" ref="W13" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(8:8)))," ")</f>
@@ -28048,7 +28059,7 @@
         <f t="array" aca="1" ref="AR13" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(8:8)))," ")</f>
         <v>3</v>
       </c>
-      <c r="AS13" s="302">
+      <c r="AS13" s="266">
         <v>2</v>
       </c>
       <c r="AT13" t="str">
@@ -28125,14 +28136,14 @@
       </c>
       <c r="T14" t="str">
         <f t="array" aca="1" ref="T14" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(9:9)))," ")</f>
-        <v>Forward Lookout</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U14" t="s">
         <v>212</v>
       </c>
       <c r="V14" t="str">
         <f t="array" aca="1" ref="V14" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T14,COUNTIF(T$6:T$55,T14)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U14,COUNTIF(U$6:U$55,U14)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>9-9</v>
+        <v>E-E</v>
       </c>
       <c r="W14" t="str">
         <f t="array" aca="1" ref="W14" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(9:9)))," ")</f>
@@ -28206,7 +28217,7 @@
         <f t="array" aca="1" ref="AR14" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(9:9)))," ")</f>
         <v>6</v>
       </c>
-      <c r="AS14" s="302">
+      <c r="AS14" s="266">
         <v>3</v>
       </c>
       <c r="AT14" t="str">
@@ -28283,14 +28294,14 @@
       </c>
       <c r="T15" t="str">
         <f t="array" aca="1" ref="T15" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(10:10)))," ")</f>
-        <v>Emergency Pump</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U15" t="s">
         <v>216</v>
       </c>
       <c r="V15" t="str">
         <f t="array" aca="1" ref="V15" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T15,COUNTIF(T$6:T$55,T15)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U15,COUNTIF(U$6:U$55,U15)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>10-10</v>
+        <v>E-E</v>
       </c>
       <c r="W15" t="str">
         <f t="array" aca="1" ref="W15" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(10:10)))," ")</f>
@@ -28364,7 +28375,7 @@
         <f t="array" aca="1" ref="AR15" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(10:10)))," ")</f>
         <v>2</v>
       </c>
-      <c r="AS15" s="302">
+      <c r="AS15" s="266">
         <v>4</v>
       </c>
       <c r="AT15" t="str">
@@ -28438,14 +28449,14 @@
       </c>
       <c r="T16" t="str">
         <f t="array" aca="1" ref="T16" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(11:11)))," ")</f>
-        <v>HDCT</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U16" t="s">
         <v>149</v>
       </c>
       <c r="V16" t="str">
         <f t="array" aca="1" ref="V16" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T16,COUNTIF(T$6:T$55,T16)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U16,COUNTIF(U$6:U$55,U16)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>5-5</v>
+        <v>E-E</v>
       </c>
       <c r="W16" t="str">
         <f t="array" aca="1" ref="W16" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(11:11)))," ")</f>
@@ -28519,7 +28530,7 @@
         <f t="array" aca="1" ref="AR16" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(11:11)))," ")</f>
         <v>5</v>
       </c>
-      <c r="AS16" s="302">
+      <c r="AS16" s="266">
         <v>5</v>
       </c>
       <c r="AT16" t="str">
@@ -28593,14 +28604,14 @@
       </c>
       <c r="T17" t="str">
         <f t="array" aca="1" ref="T17" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(12:12)))," ")</f>
-        <v>DC Party/Emerg.Str.</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U17" t="s">
         <v>243</v>
       </c>
       <c r="V17" t="str">
         <f t="array" aca="1" ref="V17" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T17,COUNTIF(T$6:T$55,T17)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U17,COUNTIF(U$6:U$55,U17)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>12-12</v>
+        <v>E-E</v>
       </c>
       <c r="W17" t="str">
         <f t="array" aca="1" ref="W17" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(12:12)))," ")</f>
@@ -28674,7 +28685,7 @@
         <f t="array" aca="1" ref="AR17" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,AS$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(12:12)))," ")</f>
         <v>1</v>
       </c>
-      <c r="AS17" s="302">
+      <c r="AS17" s="266">
         <v>6</v>
       </c>
       <c r="AT17" t="str">
@@ -28748,14 +28759,14 @@
       </c>
       <c r="T18" t="str">
         <f t="array" aca="1" ref="T18" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(13:13)))," ")</f>
-        <v>Emerg.Str.</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U18" t="s">
         <v>247</v>
       </c>
       <c r="V18" t="str">
         <f t="array" aca="1" ref="V18" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T18,COUNTIF(T$6:T$55,T18)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U18,COUNTIF(U$6:U$55,U18)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>13-13</v>
+        <v>E-E</v>
       </c>
       <c r="W18" t="str">
         <f t="array" aca="1" ref="W18" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(13:13)))," ")</f>
@@ -28900,14 +28911,14 @@
       </c>
       <c r="T19" t="str">
         <f t="array" aca="1" ref="T19" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(14:14)))," ")</f>
-        <v xml:space="preserve">DC Party/Radio </v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U19" t="s">
         <v>250</v>
       </c>
       <c r="V19" t="str">
         <f t="array" aca="1" ref="V19" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T19,COUNTIF(T$6:T$55,T19)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U19,COUNTIF(U$6:U$55,U19)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>14-14</v>
+        <v>E-E</v>
       </c>
       <c r="W19" t="str">
         <f t="array" aca="1" ref="W19" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(14:14)))," ")</f>
@@ -29049,14 +29060,14 @@
       </c>
       <c r="T20" t="str">
         <f t="array" aca="1" ref="T20" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(15:15)))," ")</f>
-        <v>Damage Control</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U20" t="s">
         <v>196</v>
       </c>
       <c r="V20" t="str">
         <f t="array" aca="1" ref="V20" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T20,COUNTIF(T$6:T$55,T20)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U20,COUNTIF(U$6:U$55,U20)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>7-7</v>
+        <v>E-E</v>
       </c>
       <c r="W20" t="str">
         <f t="array" aca="1" ref="W20" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(15:15)))," ")</f>
@@ -29198,14 +29209,14 @@
       </c>
       <c r="T21" t="str">
         <f t="array" aca="1" ref="T21" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(16:16)))," ")</f>
-        <v>OOW/Fix/Radio</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U21" t="s">
         <v>271</v>
       </c>
       <c r="V21" t="str">
         <f t="array" aca="1" ref="V21" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T21,COUNTIF(T$6:T$55,T21)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U21,COUNTIF(U$6:U$55,U21)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>16-16</v>
+        <v>E-E</v>
       </c>
       <c r="W21" t="str">
         <f t="array" aca="1" ref="W21" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(16:16)))," ")</f>
@@ -29347,14 +29358,14 @@
       </c>
       <c r="T22" t="str">
         <f t="array" aca="1" ref="T22" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(17:17)))," ")</f>
-        <v>Qtr.deck</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U22" t="s">
         <v>278</v>
       </c>
       <c r="V22" t="str">
         <f t="array" aca="1" ref="V22" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T22,COUNTIF(T$6:T$55,T22)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U22,COUNTIF(U$6:U$55,U22)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>17-17</v>
+        <v>E-E</v>
       </c>
       <c r="W22" t="str">
         <f t="array" aca="1" ref="W22" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(17:17)))," ")</f>
@@ -29493,14 +29504,14 @@
       </c>
       <c r="T23" t="str">
         <f t="array" aca="1" ref="T23" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(18:18)))," ")</f>
-        <v>HDCT Control</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U23" t="s">
         <v>282</v>
       </c>
       <c r="V23" t="str">
         <f t="array" aca="1" ref="V23" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T23,COUNTIF(T$6:T$55,T23)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U23,COUNTIF(U$6:U$55,U23)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>18-18</v>
+        <v>E-E</v>
       </c>
       <c r="W23" t="str">
         <f t="array" aca="1" ref="W23" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(18:18)))," ")</f>
@@ -29630,14 +29641,14 @@
       </c>
       <c r="T24" t="str">
         <f t="array" aca="1" ref="T24" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(19:19)))," ")</f>
-        <v>DC Party/Emerg.Str.</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U24" t="s">
         <v>243</v>
       </c>
       <c r="V24" t="str">
         <f t="array" aca="1" ref="V24" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T24,COUNTIF(T$6:T$55,T24)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U24,COUNTIF(U$6:U$55,U24)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>12-12</v>
+        <v>E-E</v>
       </c>
       <c r="W24" t="str">
         <f t="array" aca="1" ref="W24" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(19:19)))," ")</f>
@@ -29767,14 +29778,14 @@
       </c>
       <c r="T25" t="str">
         <f t="array" aca="1" ref="T25" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(20:20)))," ")</f>
-        <v xml:space="preserve">DC Party/Emerg. Str. </v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U25" t="s">
         <v>296</v>
       </c>
       <c r="V25" t="str">
         <f t="array" aca="1" ref="V25" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T25,COUNTIF(T$6:T$55,T25)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U25,COUNTIF(U$6:U$55,U25)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>20-20</v>
+        <v>E-E</v>
       </c>
       <c r="W25" t="str">
         <f t="array" aca="1" ref="W25" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(20:20)))," ")</f>
@@ -29904,14 +29915,14 @@
       </c>
       <c r="T26" t="str">
         <f t="array" aca="1" ref="T26" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(21:21)))," ")</f>
-        <v>HDCT</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U26" t="s">
         <v>149</v>
       </c>
       <c r="V26" t="str">
         <f t="array" aca="1" ref="V26" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T26,COUNTIF(T$6:T$55,T26)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U26,COUNTIF(U$6:U$55,U26)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>5-5</v>
+        <v>E-E</v>
       </c>
       <c r="W26" t="str">
         <f t="array" aca="1" ref="W26" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(21:21)))," ")</f>
@@ -30041,14 +30052,14 @@
       </c>
       <c r="T27" t="str">
         <f t="array" aca="1" ref="T27" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(22:22)))," ")</f>
-        <v>Emerg.Str.</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U27" t="s">
         <v>247</v>
       </c>
       <c r="V27" t="str">
         <f t="array" aca="1" ref="V27" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T27,COUNTIF(T$6:T$55,T27)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U27,COUNTIF(U$6:U$55,U27)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>13-13</v>
+        <v>E-E</v>
       </c>
       <c r="W27" t="str">
         <f t="array" aca="1" ref="W27" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(22:22)))," ")</f>
@@ -30175,14 +30186,14 @@
       </c>
       <c r="T28" t="str">
         <f t="array" aca="1" ref="T28" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(23:23)))," ")</f>
-        <v>Captain's Runner</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U28" t="s">
         <v>311</v>
       </c>
       <c r="V28" t="str">
         <f t="array" aca="1" ref="V28" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T28,COUNTIF(T$6:T$55,T28)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U28,COUNTIF(U$6:U$55,U28)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>23-23</v>
+        <v>E-E</v>
       </c>
       <c r="W28" t="str">
         <f t="array" aca="1" ref="W28" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(23:23)))," ")</f>
@@ -30309,14 +30320,14 @@
       </c>
       <c r="T29" t="str">
         <f t="array" aca="1" ref="T29" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(24:24)))," ")</f>
-        <v>Emerg.Str.</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U29" t="s">
         <v>247</v>
       </c>
       <c r="V29" t="str">
         <f t="array" aca="1" ref="V29" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T29,COUNTIF(T$6:T$55,T29)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U29,COUNTIF(U$6:U$55,U29)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>13-13</v>
+        <v>E-E</v>
       </c>
       <c r="W29" t="str">
         <f t="array" aca="1" ref="W29" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(24:24)))," ")</f>
@@ -30440,14 +30451,14 @@
       </c>
       <c r="T30" t="str">
         <f t="array" aca="1" ref="T30" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(25:25)))," ")</f>
-        <v>Stern Lookout</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U30" t="s">
         <v>317</v>
       </c>
       <c r="V30" t="str">
         <f t="array" aca="1" ref="V30" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T30,COUNTIF(T$6:T$55,T30)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U30,COUNTIF(U$6:U$55,U30)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>25-25</v>
+        <v>E-E</v>
       </c>
       <c r="W30" t="str">
         <f t="array" aca="1" ref="W30" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(25:25)))," ")</f>
@@ -30568,14 +30579,14 @@
       </c>
       <c r="T31" t="str">
         <f t="array" aca="1" ref="T31" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,U$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(26:26)))," ")</f>
-        <v>Helmsman</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="U31" t="s">
         <v>319</v>
       </c>
       <c r="V31" t="str">
         <f t="array" aca="1" ref="V31" ca="1">CONCATENATE(IFERROR(MATCH(CONCATENATE(T31,COUNTIF(T$6:T$55,T31)),CONCATENATE(U$6:U$55,COUNTIF(U$6:U$55,U$6:U$55)),0),"E"),"-",IFERROR(MATCH(CONCATENATE(U31,COUNTIF(U$6:U$55,U31)),CONCATENATE(T$6:T$55,COUNTIF(T$6:T$55,T$6:T$55)),0),"E"))</f>
-        <v>26-26</v>
+        <v>E-E</v>
       </c>
       <c r="W31" t="str">
         <f t="array" aca="1" ref="W31" ca="1">IFERROR(INDEX(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1),SMALL(IF(TRIM(OFFSET(WatchBillMarker,WatchBillStartOffset,X$3-1,maxValidationSize,1))&lt;&gt;"",ROW(OFFSET($A$1,0,0,maxValidationSize,1))),ROW(26:26)))," ")</f>
@@ -33758,47 +33769,47 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI6:AI55">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="22" priority="9">
       <formula>ISNUMBER(SEARCH("E-*",AK6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ6:AJ55">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="21" priority="8">
       <formula>ISNUMBER(SEARCH("*-E",AK6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL6:AL55">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="20" priority="7">
       <formula>ISNUMBER(SEARCH("E-*",AN6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM12:AM55">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="19" priority="6">
       <formula>ISNUMBER(SEARCH("*-E",AN12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO6:AO55">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="18" priority="5">
       <formula>ISNUMBER(SEARCH("E-*",AQ6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP12:AP55">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="17" priority="4">
       <formula>ISNUMBER(SEARCH("*-E",AQ12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR6:AR55">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>ISNUMBER(SEARCH("E-*",AT6))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS18:AS55">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>ISNUMBER(SEARCH("*-E",AT18))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM6:AM11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>ISNUMBER(SEARCH("*-E",AN6))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36642,78 +36653,78 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A123:E124 A122 C122:E122 A93:E94 A92 C92:E92 A63:E64 A62 C62:E62 A90:E91 A120:E121 A1:E61 B65:E89 B95:E119 A150:E1048576 B125:E149">
-    <cfRule type="containsErrors" dxfId="22" priority="18">
+    <cfRule type="containsErrors" dxfId="13" priority="18">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A123:E124 A122 C122:E122 A93:E94 A92 C92:E92 A63:E64 A62 C62:E62 A90:E91 A120:E121 A1:E61 B65:E89 B95:E119 B125:E149">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125:A149">
-    <cfRule type="containsErrors" dxfId="20" priority="8">
+    <cfRule type="containsErrors" dxfId="11" priority="8">
       <formula>ISERROR(A125)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125:A149">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:A119">
-    <cfRule type="containsErrors" dxfId="18" priority="10">
+    <cfRule type="containsErrors" dxfId="9" priority="10">
       <formula>ISERROR(A95)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A95:A119">
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A89">
-    <cfRule type="containsErrors" dxfId="16" priority="12">
+    <cfRule type="containsErrors" dxfId="7" priority="12">
       <formula>ISERROR(A65)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A89">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="containsErrors" dxfId="14" priority="6">
+    <cfRule type="containsErrors" dxfId="5" priority="6">
       <formula>ISERROR(B62)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="containsErrors" dxfId="12" priority="4">
+    <cfRule type="containsErrors" dxfId="3" priority="4">
       <formula>ISERROR(B92)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B92">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsErrors" dxfId="10" priority="2">
+    <cfRule type="containsErrors" dxfId="1" priority="2">
       <formula>ISERROR(B122)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0</formula>
       <formula>0</formula>
     </cfRule>
@@ -51365,10 +51376,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004A22A9A259F8314EB0888DA436BC1633" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4d466b61c19b9dd55e4122cf2dbe651f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d0b0c353-4067-4535-9b14-47b38980fe00" xmlns:ns3="5180a70f-888b-4c84-b9d3-a2cb8a9a6446" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afc1e0e032a009c68d4d4dff436b45db" ns2:_="" ns3:_="">
     <xsd:import namespace="d0b0c353-4067-4535-9b14-47b38980fe00"/>
@@ -51567,22 +51593,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389A6EC6-B0F1-46AA-8481-0C5A9EF26B55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EBD666A-44E4-417E-BCC9-3F6A5E2E6ECF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEA6280E-ABD1-4973-B7BC-D3149EE7866B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -51590,7 +51618,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67342A27-A527-4041-90AA-A84D4F91AD9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -51607,21 +51635,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{389A6EC6-B0F1-46AA-8481-0C5A9EF26B55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EBD666A-44E4-417E-BCC9-3F6A5E2E6ECF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>